<commit_message>
ported PIR to TM4C frame
</commit_message>
<xml_diff>
--- a/SecSys_TM4C/SecSys.xlsx
+++ b/SecSys_TM4C/SecSys.xlsx
@@ -201,13 +201,13 @@
     <t>GPIO Input</t>
   </si>
   <si>
-    <t>SIG</t>
-  </si>
-  <si>
     <t>Rising edge interrupt for PIR A trigger</t>
   </si>
   <si>
     <t>Rising edge interrupt for PIR B trigger</t>
+  </si>
+  <si>
+    <t>OUT</t>
   </si>
 </sst>
 </file>
@@ -361,9 +361,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -371,22 +368,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -684,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -719,583 +719,583 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="3.75" customHeight="1">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4" t="s">
+      <c r="A4" s="12"/>
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="5" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="12"/>
+      <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4" t="s">
+      <c r="A6" s="12"/>
+      <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="12"/>
+      <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="6"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4" t="s">
+      <c r="A8" s="12"/>
+      <c r="B8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4" t="s">
+      <c r="A9" s="12"/>
+      <c r="B9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4" t="s">
+      <c r="A10" s="12"/>
+      <c r="B10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:7" ht="3.75" customHeight="1">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4" t="s">
+      <c r="A13" s="12"/>
+      <c r="B13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4" t="s">
+      <c r="A14" s="12"/>
+      <c r="B14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4" t="s">
+      <c r="A15" s="12"/>
+      <c r="B15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4" t="s">
+      <c r="A16" s="12"/>
+      <c r="B16" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="3"/>
-      <c r="B17" s="4" t="s">
+      <c r="A17" s="12"/>
+      <c r="B17" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="3"/>
-      <c r="B18" s="4" t="s">
+      <c r="A18" s="12"/>
+      <c r="B18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" ht="3.75" customHeight="1">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="3"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="3"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="3"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
+      <c r="A23" s="12"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="3"/>
-      <c r="B24" s="15" t="s">
+      <c r="A24" s="12"/>
+      <c r="B24" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="3"/>
-      <c r="B25" s="15" t="s">
+      <c r="A25" s="12"/>
+      <c r="B25" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="3"/>
-      <c r="B26" s="15" t="s">
+      <c r="A26" s="12"/>
+      <c r="B26" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="D26" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E26" s="15" t="s">
+      <c r="E26" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="12"/>
+      <c r="B27" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="F26" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="G26" s="4" t="s">
+      <c r="F27" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G27" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="3"/>
-      <c r="B27" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="F27" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="G27" s="4" t="s">
+    <row r="28" spans="1:7" ht="3.75" customHeight="1">
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="12"/>
+      <c r="B30" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="12"/>
+      <c r="B31" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="12"/>
+      <c r="B32" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="12"/>
+      <c r="B33" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G33" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="3.75" customHeight="1">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="3"/>
-      <c r="B30" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="3"/>
-      <c r="B31" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="3"/>
-      <c r="B32" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="3"/>
-      <c r="B33" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C33" s="6" t="s">
+    <row r="34" spans="1:7">
+      <c r="A34" s="12"/>
+      <c r="B34" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F34" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D33" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G33" s="4" t="s">
+      <c r="G34" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
-      <c r="A34" s="3"/>
-      <c r="B34" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
     <row r="35" spans="1:7" ht="3.75" customHeight="1">
-      <c r="A35" s="12"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
     </row>
     <row r="36" spans="1:7" ht="15" customHeight="1">
       <c r="A36" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="B36" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
     </row>
     <row r="37" spans="1:7" ht="15" customHeight="1">
       <c r="A37" s="14"/>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
     </row>
     <row r="38" spans="1:7" ht="15" customHeight="1">
       <c r="A38" s="14"/>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C38" s="8"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
     </row>
     <row r="39" spans="1:7" ht="15" customHeight="1">
       <c r="A39" s="14"/>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C39" s="8"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="14"/>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="8"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="14"/>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="8"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
     </row>
     <row r="42" spans="1:7" ht="3.75" customHeight="1">
-      <c r="A42" s="12"/>
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="12"/>
+      <c r="A42" s="10"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="3"/>
-      <c r="B44" s="5" t="s">
+      <c r="A44" s="12"/>
+      <c r="B44" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="3"/>
-      <c r="B45" s="11" t="s">
+      <c r="A45" s="12"/>
+      <c r="B45" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="3"/>
-      <c r="B46" s="7" t="s">
+      <c r="A46" s="12"/>
+      <c r="B46" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
-      <c r="G46" s="4"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="3"/>
-      <c r="B47" s="4" t="s">
+      <c r="A47" s="12"/>
+      <c r="B47" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
     </row>
     <row r="48" spans="1:7" ht="3.75" customHeight="1">
-      <c r="A48" s="12"/>
-      <c r="B48" s="12"/>
-      <c r="C48" s="12"/>
-      <c r="D48" s="12"/>
-      <c r="E48" s="12"/>
-      <c r="F48" s="12"/>
-      <c r="G48" s="12"/>
+      <c r="A48" s="10"/>
+      <c r="B48" s="10"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="B20:G23"/>
+    <mergeCell ref="A29:A34"/>
     <mergeCell ref="A43:A47"/>
     <mergeCell ref="A36:A41"/>
     <mergeCell ref="A3:A10"/>
     <mergeCell ref="A12:A18"/>
     <mergeCell ref="A20:A27"/>
-    <mergeCell ref="B20:G23"/>
-    <mergeCell ref="A29:A34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>

</xml_diff>

<commit_message>
develop driver for HX711 to sample data from loadcell
</commit_message>
<xml_diff>
--- a/SecSys_TM4C/SecSys.xlsx
+++ b/SecSys_TM4C/SecSys.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -22,7 +22,7 @@
     <definedName name="R_4">'[1]Light sensor #1'!$D$4</definedName>
     <definedName name="V_in">'[1]Light sensor #1'!$B$5</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -411,23 +411,23 @@
     </r>
   </si>
   <si>
-    <t>Load cell input 1</t>
-  </si>
-  <si>
-    <t>Load cell input 2</t>
-  </si>
-  <si>
-    <t>Temperature sensor input</t>
+    <t>Load cell input (DOUT)</t>
+  </si>
+  <si>
+    <t>Load cell output (SLK)</t>
+  </si>
+  <si>
+    <t>Temperature sensor in/out (onewire)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -711,18 +711,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -746,17 +734,37 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="To Do!!!"/>
@@ -861,7 +869,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -893,9 +901,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -927,6 +953,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1102,14 +1146,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
       <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
@@ -1119,7 +1163,7 @@
     <col min="7" max="7" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1139,7 +1183,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="3.75" customHeight="1">
+    <row r="2" spans="1:7" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -1148,8 +1192,8 @@
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="34" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1171,8 +1215,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="13"/>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="34"/>
       <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
@@ -1192,8 +1236,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="13"/>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="34"/>
       <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
@@ -1203,8 +1247,8 @@
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="13"/>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="34"/>
       <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
@@ -1214,8 +1258,8 @@
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="13"/>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="34"/>
       <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
@@ -1225,8 +1269,8 @@
       <c r="F7" s="3"/>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="13"/>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="34"/>
       <c r="B8" s="3" t="s">
         <v>12</v>
       </c>
@@ -1236,8 +1280,8 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="13"/>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="34"/>
       <c r="B9" s="3" t="s">
         <v>13</v>
       </c>
@@ -1247,8 +1291,8 @@
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="13"/>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="34"/>
       <c r="B10" s="3" t="s">
         <v>14</v>
       </c>
@@ -1258,7 +1302,7 @@
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:7" ht="3.75" customHeight="1">
+    <row r="11" spans="1:7" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
@@ -1267,8 +1311,8 @@
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
     </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="13" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="34" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -1280,8 +1324,8 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="13"/>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="34"/>
       <c r="B13" s="3" t="s">
         <v>17</v>
       </c>
@@ -1291,8 +1335,8 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="13"/>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="34"/>
       <c r="B14" s="3" t="s">
         <v>18</v>
       </c>
@@ -1302,8 +1346,8 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="13"/>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="34"/>
       <c r="B15" s="3" t="s">
         <v>19</v>
       </c>
@@ -1313,8 +1357,8 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="13"/>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="34"/>
       <c r="B16" s="3" t="s">
         <v>21</v>
       </c>
@@ -1324,8 +1368,8 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="13"/>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="34"/>
       <c r="B17" s="3" t="s">
         <v>22</v>
       </c>
@@ -1335,8 +1379,8 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="13"/>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="34"/>
       <c r="B18" s="3" t="s">
         <v>23</v>
       </c>
@@ -1346,7 +1390,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:7" ht="3.75" customHeight="1">
+    <row r="19" spans="1:7" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
@@ -1355,48 +1399,48 @@
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
     </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="13" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="13"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="13"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="13"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="13"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="33"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="34"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="34"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="33"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="34"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="33"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="34"/>
       <c r="B24" s="11" t="s">
         <v>26</v>
       </c>
@@ -1406,8 +1450,8 @@
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
     </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="13"/>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="34"/>
       <c r="B25" s="11" t="s">
         <v>27</v>
       </c>
@@ -1417,8 +1461,8 @@
       <c r="F25" s="11"/>
       <c r="G25" s="11"/>
     </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="13"/>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="34"/>
       <c r="B26" s="11" t="s">
         <v>28</v>
       </c>
@@ -1438,8 +1482,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="13"/>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="34"/>
       <c r="B27" s="11" t="s">
         <v>29</v>
       </c>
@@ -1459,7 +1503,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="3.75" customHeight="1">
+    <row r="28" spans="1:7" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
@@ -1468,8 +1512,8 @@
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
     </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="13" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="34" t="s">
         <v>30</v>
       </c>
       <c r="B29" s="5" t="s">
@@ -1481,8 +1525,8 @@
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
     </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="13"/>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="34"/>
       <c r="B30" s="5" t="s">
         <v>32</v>
       </c>
@@ -1492,8 +1536,8 @@
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
     </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="13"/>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="34"/>
       <c r="B31" s="5" t="s">
         <v>33</v>
       </c>
@@ -1503,8 +1547,8 @@
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
     </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="13"/>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="34"/>
       <c r="B32" s="5" t="s">
         <v>34</v>
       </c>
@@ -1514,8 +1558,8 @@
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
     </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="13"/>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="34"/>
       <c r="B33" s="8" t="s">
         <v>35</v>
       </c>
@@ -1535,8 +1579,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
-      <c r="A34" s="13"/>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="34"/>
       <c r="B34" s="3" t="s">
         <v>36</v>
       </c>
@@ -1556,7 +1600,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="3.75" customHeight="1">
+    <row r="35" spans="1:7" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10"/>
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
@@ -1565,8 +1609,8 @@
       <c r="F35" s="10"/>
       <c r="G35" s="10"/>
     </row>
-    <row r="36" spans="1:7" ht="15" customHeight="1">
-      <c r="A36" s="14" t="s">
+    <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="35" t="s">
         <v>37</v>
       </c>
       <c r="B36" s="8" t="s">
@@ -1578,8 +1622,8 @@
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
     </row>
-    <row r="37" spans="1:7" ht="15" customHeight="1">
-      <c r="A37" s="15"/>
+    <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="36"/>
       <c r="B37" s="3" t="s">
         <v>39</v>
       </c>
@@ -1593,8 +1637,8 @@
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
     </row>
-    <row r="38" spans="1:7" ht="15" customHeight="1">
-      <c r="A38" s="15"/>
+    <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="36"/>
       <c r="B38" s="3" t="s">
         <v>40</v>
       </c>
@@ -1608,8 +1652,8 @@
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
     </row>
-    <row r="39" spans="1:7" ht="15" customHeight="1">
-      <c r="A39" s="15"/>
+    <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="36"/>
       <c r="B39" s="3" t="s">
         <v>41</v>
       </c>
@@ -1623,8 +1667,8 @@
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
     </row>
-    <row r="40" spans="1:7">
-      <c r="A40" s="15"/>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="36"/>
       <c r="B40" s="3" t="s">
         <v>56</v>
       </c>
@@ -1634,8 +1678,8 @@
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
     </row>
-    <row r="41" spans="1:7">
-      <c r="A41" s="15"/>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="36"/>
       <c r="B41" s="3" t="s">
         <v>57</v>
       </c>
@@ -1645,7 +1689,7 @@
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
     </row>
-    <row r="42" spans="1:7" ht="3.75" customHeight="1">
+    <row r="42" spans="1:7" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
@@ -1654,8 +1698,8 @@
       <c r="F42" s="10"/>
       <c r="G42" s="10"/>
     </row>
-    <row r="43" spans="1:7">
-      <c r="A43" s="13" t="s">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="34" t="s">
         <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
@@ -1667,8 +1711,8 @@
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
     </row>
-    <row r="44" spans="1:7">
-      <c r="A44" s="13"/>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="34"/>
       <c r="B44" s="4" t="s">
         <v>44</v>
       </c>
@@ -1678,8 +1722,8 @@
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
     </row>
-    <row r="45" spans="1:7">
-      <c r="A45" s="13"/>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="34"/>
       <c r="B45" s="9" t="s">
         <v>45</v>
       </c>
@@ -1689,8 +1733,8 @@
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
     </row>
-    <row r="46" spans="1:7">
-      <c r="A46" s="13"/>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="34"/>
       <c r="B46" s="6" t="s">
         <v>46</v>
       </c>
@@ -1700,8 +1744,8 @@
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
     </row>
-    <row r="47" spans="1:7">
-      <c r="A47" s="13"/>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="34"/>
       <c r="B47" s="3" t="s">
         <v>47</v>
       </c>
@@ -1711,7 +1755,7 @@
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
     </row>
-    <row r="48" spans="1:7" ht="3.75" customHeight="1">
+    <row r="48" spans="1:7" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="10"/>
       <c r="B48" s="10"/>
       <c r="C48" s="10"/>
@@ -1736,14 +1780,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
@@ -1755,179 +1799,179 @@
     <col min="13" max="13" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="17">
+      <c r="B1" s="13">
         <v>0.1</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="19">
+      <c r="D1" s="15">
         <f>B1*10^3</f>
         <v>100</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="F1" s="20">
+      <c r="F1" s="16">
         <f>D1*10^3</f>
         <v>100000</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="21">
+      <c r="H1" s="17">
         <f>D1*10^6</f>
         <v>100000000</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="17" t="s">
         <v>68</v>
       </c>
       <c r="S1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
-      <c r="A2" s="16" t="s">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="18">
+      <c r="B2" s="14">
         <f>1/B1</f>
         <v>10</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="D2" s="19">
+      <c r="D2" s="15">
         <f>B2/10^3</f>
         <v>0.01</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="F2" s="20">
+      <c r="F2" s="16">
         <f>B2/10^6</f>
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="H2" s="21">
+      <c r="H2" s="17">
         <f>F2/10^3</f>
         <v>1E-8</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="L2" s="22" t="s">
+      <c r="L2" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="M2" s="22" t="s">
+      <c r="M2" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-    </row>
-    <row r="3" spans="1:19">
-      <c r="A3" s="16" t="s">
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="B3" s="23">
+      <c r="B3" s="19">
         <f>(F3*10^6)</f>
         <v>80000000</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D3" s="20">
         <f>B3/10^3</f>
         <v>80000</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="13">
         <v>80</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="H3" s="26">
+      <c r="H3" s="22">
         <f>F3/10^3</f>
         <v>0.08</v>
       </c>
-      <c r="I3" s="26" t="s">
+      <c r="I3" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="L3" s="22" t="s">
+      <c r="L3" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="M3" s="22" t="s">
+      <c r="M3" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="N3" s="22"/>
-      <c r="O3" s="22"/>
-    </row>
-    <row r="4" spans="1:19">
-      <c r="A4" s="16" t="s">
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="B4" s="27">
+      <c r="B4" s="23">
         <f>1/B3</f>
         <v>1.2499999999999999E-8</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="D4" s="28">
+      <c r="D4" s="24">
         <f>B4*10^3</f>
         <v>1.2499999999999999E-5</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="F4" s="29">
+      <c r="F4" s="25">
         <f>D4*10^3</f>
         <v>1.2499999999999999E-2</v>
       </c>
-      <c r="G4" s="29" t="s">
+      <c r="G4" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="H4" s="30">
+      <c r="H4" s="26">
         <f>B4*10^9</f>
         <v>12.5</v>
       </c>
-      <c r="I4" s="30" t="s">
+      <c r="I4" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="L4" s="22" t="s">
+      <c r="L4" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="M4" s="22" t="s">
+      <c r="M4" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="N4" s="22"/>
-      <c r="O4" s="22"/>
-    </row>
-    <row r="5" spans="1:19">
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="H5">
         <f>1/B3*10^9</f>
         <v>12.5</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
-      <c r="A6" s="31" t="s">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="32">
+      <c r="B6" s="28">
         <f>(H1/H4)-1</f>
         <v>7999999</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
       <c r="E6" t="s">
         <v>84</v>
       </c>
@@ -1936,11 +1980,11 @@
         <v>312.5</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
-      <c r="A7" s="31" t="s">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="B7" s="32" t="str">
+      <c r="B7" s="28" t="str">
         <f>DEC2HEX(B6)</f>
         <v>7A11FF</v>
       </c>
@@ -1950,9 +1994,9 @@
       <c r="F7">
         <v>5000</v>
       </c>
-      <c r="H7" s="34"/>
-    </row>
-    <row r="8" spans="1:19">
+      <c r="H7" s="30"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
         <v>87</v>
       </c>
@@ -1960,21 +2004,21 @@
         <v>16000</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
-      <c r="A9" s="35" t="s">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="31" t="s">
         <v>88</v>
       </c>
       <c r="B9">
         <v>7999900</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="15.75">
-      <c r="A12" s="36" t="s">
+    <row r="12" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="32" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="15.75">
-      <c r="A13" s="36" t="s">
+    <row r="13" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="32" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1985,24 +2029,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
work on receive SMS functionality
</commit_message>
<xml_diff>
--- a/SecSys_TM4C/SecSys.xlsx
+++ b/SecSys_TM4C/SecSys.xlsx
@@ -426,10 +426,6 @@
     <t>PIR</t>
   </si>
   <si>
-    <t>Shield PIR sensor (with connection to GND)
-Large capacitor on PIR power supply</t>
-  </si>
-  <si>
     <t>Temperature Sensor:</t>
   </si>
   <si>
@@ -449,6 +445,42 @@
   </si>
   <si>
     <t>Trigger SMS warning</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Shield PIR sensor (with connection to GND)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Large capacitor on PIR power supply
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Trigger ALARM only after X nr of PIR triggers within Y seconds</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -458,7 +490,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -529,6 +561,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -845,6 +885,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -871,9 +914,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1877,800 +1917,800 @@
   <dimension ref="A1:U33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W15" sqref="W15"/>
+      <selection activeCell="O23" sqref="O23:U23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:21">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46" t="s">
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="37"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="37"/>
+    </row>
+    <row r="2" spans="1:21">
+      <c r="A2" s="38" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="39"/>
+      <c r="U2" s="40"/>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="A3" s="41"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="43"/>
+      <c r="O3" s="41"/>
+      <c r="P3" s="42"/>
+      <c r="Q3" s="42"/>
+      <c r="R3" s="42"/>
+      <c r="S3" s="42"/>
+      <c r="T3" s="42"/>
+      <c r="U3" s="43"/>
+    </row>
+    <row r="4" spans="1:21">
+      <c r="A4" s="41"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="43"/>
+      <c r="O4" s="41"/>
+      <c r="P4" s="42"/>
+      <c r="Q4" s="42"/>
+      <c r="R4" s="42"/>
+      <c r="S4" s="42"/>
+      <c r="T4" s="42"/>
+      <c r="U4" s="43"/>
+    </row>
+    <row r="5" spans="1:21">
+      <c r="A5" s="41"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="42"/>
+      <c r="L5" s="42"/>
+      <c r="M5" s="42"/>
+      <c r="N5" s="43"/>
+      <c r="O5" s="41"/>
+      <c r="P5" s="42"/>
+      <c r="Q5" s="42"/>
+      <c r="R5" s="42"/>
+      <c r="S5" s="42"/>
+      <c r="T5" s="42"/>
+      <c r="U5" s="43"/>
+    </row>
+    <row r="6" spans="1:21">
+      <c r="A6" s="41"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="42"/>
+      <c r="L6" s="42"/>
+      <c r="M6" s="42"/>
+      <c r="N6" s="43"/>
+      <c r="O6" s="41"/>
+      <c r="P6" s="42"/>
+      <c r="Q6" s="42"/>
+      <c r="R6" s="42"/>
+      <c r="S6" s="42"/>
+      <c r="T6" s="42"/>
+      <c r="U6" s="43"/>
+    </row>
+    <row r="7" spans="1:21">
+      <c r="A7" s="41"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="42"/>
+      <c r="J7" s="42"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="42"/>
+      <c r="M7" s="42"/>
+      <c r="N7" s="43"/>
+      <c r="O7" s="41"/>
+      <c r="P7" s="42"/>
+      <c r="Q7" s="42"/>
+      <c r="R7" s="42"/>
+      <c r="S7" s="42"/>
+      <c r="T7" s="42"/>
+      <c r="U7" s="43"/>
+    </row>
+    <row r="8" spans="1:21">
+      <c r="A8" s="41"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="42"/>
+      <c r="M8" s="42"/>
+      <c r="N8" s="43"/>
+      <c r="O8" s="41"/>
+      <c r="P8" s="42"/>
+      <c r="Q8" s="42"/>
+      <c r="R8" s="42"/>
+      <c r="S8" s="42"/>
+      <c r="T8" s="42"/>
+      <c r="U8" s="43"/>
+    </row>
+    <row r="9" spans="1:21">
+      <c r="A9" s="41"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="42"/>
+      <c r="L9" s="42"/>
+      <c r="M9" s="42"/>
+      <c r="N9" s="43"/>
+      <c r="O9" s="41"/>
+      <c r="P9" s="42"/>
+      <c r="Q9" s="42"/>
+      <c r="R9" s="42"/>
+      <c r="S9" s="42"/>
+      <c r="T9" s="42"/>
+      <c r="U9" s="43"/>
+    </row>
+    <row r="10" spans="1:21">
+      <c r="A10" s="41"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="42"/>
+      <c r="N10" s="43"/>
+      <c r="O10" s="41"/>
+      <c r="P10" s="42"/>
+      <c r="Q10" s="42"/>
+      <c r="R10" s="42"/>
+      <c r="S10" s="42"/>
+      <c r="T10" s="42"/>
+      <c r="U10" s="43"/>
+    </row>
+    <row r="11" spans="1:21">
+      <c r="A11" s="44"/>
+      <c r="B11" s="45"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="45"/>
+      <c r="J11" s="45"/>
+      <c r="K11" s="45"/>
+      <c r="L11" s="45"/>
+      <c r="M11" s="45"/>
+      <c r="N11" s="46"/>
+      <c r="O11" s="44"/>
+      <c r="P11" s="45"/>
+      <c r="Q11" s="45"/>
+      <c r="R11" s="45"/>
+      <c r="S11" s="45"/>
+      <c r="T11" s="45"/>
+      <c r="U11" s="46"/>
+    </row>
+    <row r="12" spans="1:21">
+      <c r="A12" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" s="37"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37" t="s">
+        <v>98</v>
+      </c>
+      <c r="I12" s="37"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="37"/>
+      <c r="M12" s="37"/>
+      <c r="N12" s="37"/>
+      <c r="O12" s="37"/>
+      <c r="P12" s="37"/>
+      <c r="Q12" s="37"/>
+      <c r="R12" s="37"/>
+      <c r="S12" s="37"/>
+      <c r="T12" s="37"/>
+      <c r="U12" s="37"/>
+    </row>
+    <row r="13" spans="1:21">
+      <c r="A13" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13" s="39"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="46"/>
-      <c r="S1" s="46"/>
-      <c r="T1" s="46"/>
-      <c r="U1" s="46"/>
-    </row>
-    <row r="2" spans="1:21">
-      <c r="A2" s="37" t="s">
-        <v>100</v>
-      </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="37" t="s">
-        <v>96</v>
-      </c>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="38"/>
-      <c r="R2" s="38"/>
-      <c r="S2" s="38"/>
-      <c r="T2" s="38"/>
-      <c r="U2" s="39"/>
-    </row>
-    <row r="3" spans="1:21">
-      <c r="A3" s="40"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="42"/>
-      <c r="O3" s="40"/>
-      <c r="P3" s="41"/>
-      <c r="Q3" s="41"/>
-      <c r="R3" s="41"/>
-      <c r="S3" s="41"/>
-      <c r="T3" s="41"/>
-      <c r="U3" s="42"/>
-    </row>
-    <row r="4" spans="1:21">
-      <c r="A4" s="40"/>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="41"/>
-      <c r="K4" s="41"/>
-      <c r="L4" s="41"/>
-      <c r="M4" s="41"/>
-      <c r="N4" s="42"/>
-      <c r="O4" s="40"/>
-      <c r="P4" s="41"/>
-      <c r="Q4" s="41"/>
-      <c r="R4" s="41"/>
-      <c r="S4" s="41"/>
-      <c r="T4" s="41"/>
-      <c r="U4" s="42"/>
-    </row>
-    <row r="5" spans="1:21">
-      <c r="A5" s="40"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="41"/>
-      <c r="K5" s="41"/>
-      <c r="L5" s="41"/>
-      <c r="M5" s="41"/>
-      <c r="N5" s="42"/>
-      <c r="O5" s="40"/>
-      <c r="P5" s="41"/>
-      <c r="Q5" s="41"/>
-      <c r="R5" s="41"/>
-      <c r="S5" s="41"/>
-      <c r="T5" s="41"/>
-      <c r="U5" s="42"/>
-    </row>
-    <row r="6" spans="1:21">
-      <c r="A6" s="40"/>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="41"/>
-      <c r="L6" s="41"/>
-      <c r="M6" s="41"/>
-      <c r="N6" s="42"/>
-      <c r="O6" s="40"/>
-      <c r="P6" s="41"/>
-      <c r="Q6" s="41"/>
-      <c r="R6" s="41"/>
-      <c r="S6" s="41"/>
-      <c r="T6" s="41"/>
-      <c r="U6" s="42"/>
-    </row>
-    <row r="7" spans="1:21">
-      <c r="A7" s="40"/>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="41"/>
-      <c r="M7" s="41"/>
-      <c r="N7" s="42"/>
-      <c r="O7" s="40"/>
-      <c r="P7" s="41"/>
-      <c r="Q7" s="41"/>
-      <c r="R7" s="41"/>
-      <c r="S7" s="41"/>
-      <c r="T7" s="41"/>
-      <c r="U7" s="42"/>
-    </row>
-    <row r="8" spans="1:21">
-      <c r="A8" s="40"/>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="40"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="41"/>
-      <c r="M8" s="41"/>
-      <c r="N8" s="42"/>
-      <c r="O8" s="40"/>
-      <c r="P8" s="41"/>
-      <c r="Q8" s="41"/>
-      <c r="R8" s="41"/>
-      <c r="S8" s="41"/>
-      <c r="T8" s="41"/>
-      <c r="U8" s="42"/>
-    </row>
-    <row r="9" spans="1:21">
-      <c r="A9" s="40"/>
-      <c r="B9" s="41"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="41"/>
-      <c r="J9" s="41"/>
-      <c r="K9" s="41"/>
-      <c r="L9" s="41"/>
-      <c r="M9" s="41"/>
-      <c r="N9" s="42"/>
-      <c r="O9" s="40"/>
-      <c r="P9" s="41"/>
-      <c r="Q9" s="41"/>
-      <c r="R9" s="41"/>
-      <c r="S9" s="41"/>
-      <c r="T9" s="41"/>
-      <c r="U9" s="42"/>
-    </row>
-    <row r="10" spans="1:21">
-      <c r="A10" s="40"/>
-      <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="41"/>
-      <c r="J10" s="41"/>
-      <c r="K10" s="41"/>
-      <c r="L10" s="41"/>
-      <c r="M10" s="41"/>
-      <c r="N10" s="42"/>
-      <c r="O10" s="40"/>
-      <c r="P10" s="41"/>
-      <c r="Q10" s="41"/>
-      <c r="R10" s="41"/>
-      <c r="S10" s="41"/>
-      <c r="T10" s="41"/>
-      <c r="U10" s="42"/>
-    </row>
-    <row r="11" spans="1:21">
-      <c r="A11" s="43"/>
-      <c r="B11" s="44"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="44"/>
-      <c r="K11" s="44"/>
-      <c r="L11" s="44"/>
-      <c r="M11" s="44"/>
-      <c r="N11" s="45"/>
-      <c r="O11" s="43"/>
-      <c r="P11" s="44"/>
-      <c r="Q11" s="44"/>
-      <c r="R11" s="44"/>
-      <c r="S11" s="44"/>
-      <c r="T11" s="44"/>
-      <c r="U11" s="45"/>
-    </row>
-    <row r="12" spans="1:21">
-      <c r="A12" s="46" t="s">
-        <v>97</v>
-      </c>
-      <c r="B12" s="46"/>
-      <c r="C12" s="46"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46" t="s">
-        <v>99</v>
-      </c>
-      <c r="I12" s="46"/>
-      <c r="J12" s="46"/>
-      <c r="K12" s="46"/>
-      <c r="L12" s="46"/>
-      <c r="M12" s="46"/>
-      <c r="N12" s="46"/>
-      <c r="O12" s="46"/>
-      <c r="P12" s="46"/>
-      <c r="Q12" s="46"/>
-      <c r="R12" s="46"/>
-      <c r="S12" s="46"/>
-      <c r="T12" s="46"/>
-      <c r="U12" s="46"/>
-    </row>
-    <row r="13" spans="1:21">
-      <c r="A13" s="37" t="s">
-        <v>98</v>
-      </c>
-      <c r="B13" s="38"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="37" t="s">
-        <v>102</v>
-      </c>
-      <c r="I13" s="38"/>
-      <c r="J13" s="38"/>
-      <c r="K13" s="38"/>
-      <c r="L13" s="38"/>
-      <c r="M13" s="38"/>
-      <c r="N13" s="39"/>
-      <c r="O13" s="37"/>
-      <c r="P13" s="38"/>
-      <c r="Q13" s="38"/>
-      <c r="R13" s="38"/>
-      <c r="S13" s="38"/>
-      <c r="T13" s="38"/>
-      <c r="U13" s="39"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="39"/>
+      <c r="L13" s="39"/>
+      <c r="M13" s="39"/>
+      <c r="N13" s="40"/>
+      <c r="O13" s="38"/>
+      <c r="P13" s="39"/>
+      <c r="Q13" s="39"/>
+      <c r="R13" s="39"/>
+      <c r="S13" s="39"/>
+      <c r="T13" s="39"/>
+      <c r="U13" s="40"/>
     </row>
     <row r="14" spans="1:21">
-      <c r="A14" s="40"/>
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="41"/>
-      <c r="J14" s="41"/>
-      <c r="K14" s="41"/>
-      <c r="L14" s="41"/>
-      <c r="M14" s="41"/>
-      <c r="N14" s="42"/>
-      <c r="O14" s="40"/>
-      <c r="P14" s="41"/>
-      <c r="Q14" s="41"/>
-      <c r="R14" s="41"/>
-      <c r="S14" s="41"/>
-      <c r="T14" s="41"/>
-      <c r="U14" s="42"/>
+      <c r="A14" s="41"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="42"/>
+      <c r="K14" s="42"/>
+      <c r="L14" s="42"/>
+      <c r="M14" s="42"/>
+      <c r="N14" s="43"/>
+      <c r="O14" s="41"/>
+      <c r="P14" s="42"/>
+      <c r="Q14" s="42"/>
+      <c r="R14" s="42"/>
+      <c r="S14" s="42"/>
+      <c r="T14" s="42"/>
+      <c r="U14" s="43"/>
     </row>
     <row r="15" spans="1:21">
-      <c r="A15" s="40"/>
-      <c r="B15" s="41"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="41"/>
-      <c r="J15" s="41"/>
-      <c r="K15" s="41"/>
-      <c r="L15" s="41"/>
-      <c r="M15" s="41"/>
-      <c r="N15" s="42"/>
-      <c r="O15" s="40"/>
-      <c r="P15" s="41"/>
-      <c r="Q15" s="41"/>
-      <c r="R15" s="41"/>
-      <c r="S15" s="41"/>
-      <c r="T15" s="41"/>
-      <c r="U15" s="42"/>
+      <c r="A15" s="41"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="42"/>
+      <c r="J15" s="42"/>
+      <c r="K15" s="42"/>
+      <c r="L15" s="42"/>
+      <c r="M15" s="42"/>
+      <c r="N15" s="43"/>
+      <c r="O15" s="41"/>
+      <c r="P15" s="42"/>
+      <c r="Q15" s="42"/>
+      <c r="R15" s="42"/>
+      <c r="S15" s="42"/>
+      <c r="T15" s="42"/>
+      <c r="U15" s="43"/>
     </row>
     <row r="16" spans="1:21">
-      <c r="A16" s="40"/>
-      <c r="B16" s="41"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="41"/>
-      <c r="J16" s="41"/>
-      <c r="K16" s="41"/>
-      <c r="L16" s="41"/>
-      <c r="M16" s="41"/>
-      <c r="N16" s="42"/>
-      <c r="O16" s="40"/>
-      <c r="P16" s="41"/>
-      <c r="Q16" s="41"/>
-      <c r="R16" s="41"/>
-      <c r="S16" s="41"/>
-      <c r="T16" s="41"/>
-      <c r="U16" s="42"/>
+      <c r="A16" s="41"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
+      <c r="K16" s="42"/>
+      <c r="L16" s="42"/>
+      <c r="M16" s="42"/>
+      <c r="N16" s="43"/>
+      <c r="O16" s="41"/>
+      <c r="P16" s="42"/>
+      <c r="Q16" s="42"/>
+      <c r="R16" s="42"/>
+      <c r="S16" s="42"/>
+      <c r="T16" s="42"/>
+      <c r="U16" s="43"/>
     </row>
     <row r="17" spans="1:21">
-      <c r="A17" s="40"/>
-      <c r="B17" s="41"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="41"/>
-      <c r="J17" s="41"/>
-      <c r="K17" s="41"/>
-      <c r="L17" s="41"/>
-      <c r="M17" s="41"/>
-      <c r="N17" s="42"/>
-      <c r="O17" s="40"/>
-      <c r="P17" s="41"/>
-      <c r="Q17" s="41"/>
-      <c r="R17" s="41"/>
-      <c r="S17" s="41"/>
-      <c r="T17" s="41"/>
-      <c r="U17" s="42"/>
+      <c r="A17" s="41"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
+      <c r="K17" s="42"/>
+      <c r="L17" s="42"/>
+      <c r="M17" s="42"/>
+      <c r="N17" s="43"/>
+      <c r="O17" s="41"/>
+      <c r="P17" s="42"/>
+      <c r="Q17" s="42"/>
+      <c r="R17" s="42"/>
+      <c r="S17" s="42"/>
+      <c r="T17" s="42"/>
+      <c r="U17" s="43"/>
     </row>
     <row r="18" spans="1:21">
-      <c r="A18" s="40"/>
-      <c r="B18" s="41"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="41"/>
-      <c r="J18" s="41"/>
-      <c r="K18" s="41"/>
-      <c r="L18" s="41"/>
-      <c r="M18" s="41"/>
-      <c r="N18" s="42"/>
-      <c r="O18" s="40"/>
-      <c r="P18" s="41"/>
-      <c r="Q18" s="41"/>
-      <c r="R18" s="41"/>
-      <c r="S18" s="41"/>
-      <c r="T18" s="41"/>
-      <c r="U18" s="42"/>
+      <c r="A18" s="41"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
+      <c r="K18" s="42"/>
+      <c r="L18" s="42"/>
+      <c r="M18" s="42"/>
+      <c r="N18" s="43"/>
+      <c r="O18" s="41"/>
+      <c r="P18" s="42"/>
+      <c r="Q18" s="42"/>
+      <c r="R18" s="42"/>
+      <c r="S18" s="42"/>
+      <c r="T18" s="42"/>
+      <c r="U18" s="43"/>
     </row>
     <row r="19" spans="1:21">
-      <c r="A19" s="40"/>
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="42"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="41"/>
-      <c r="J19" s="41"/>
-      <c r="K19" s="41"/>
-      <c r="L19" s="41"/>
-      <c r="M19" s="41"/>
-      <c r="N19" s="42"/>
-      <c r="O19" s="40"/>
-      <c r="P19" s="41"/>
-      <c r="Q19" s="41"/>
-      <c r="R19" s="41"/>
-      <c r="S19" s="41"/>
-      <c r="T19" s="41"/>
-      <c r="U19" s="42"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="43"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
+      <c r="K19" s="42"/>
+      <c r="L19" s="42"/>
+      <c r="M19" s="42"/>
+      <c r="N19" s="43"/>
+      <c r="O19" s="41"/>
+      <c r="P19" s="42"/>
+      <c r="Q19" s="42"/>
+      <c r="R19" s="42"/>
+      <c r="S19" s="42"/>
+      <c r="T19" s="42"/>
+      <c r="U19" s="43"/>
     </row>
     <row r="20" spans="1:21">
-      <c r="A20" s="40"/>
-      <c r="B20" s="41"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="41"/>
-      <c r="J20" s="41"/>
-      <c r="K20" s="41"/>
-      <c r="L20" s="41"/>
-      <c r="M20" s="41"/>
-      <c r="N20" s="42"/>
-      <c r="O20" s="40"/>
-      <c r="P20" s="41"/>
-      <c r="Q20" s="41"/>
-      <c r="R20" s="41"/>
-      <c r="S20" s="41"/>
-      <c r="T20" s="41"/>
-      <c r="U20" s="42"/>
+      <c r="A20" s="41"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="42"/>
+      <c r="K20" s="42"/>
+      <c r="L20" s="42"/>
+      <c r="M20" s="42"/>
+      <c r="N20" s="43"/>
+      <c r="O20" s="41"/>
+      <c r="P20" s="42"/>
+      <c r="Q20" s="42"/>
+      <c r="R20" s="42"/>
+      <c r="S20" s="42"/>
+      <c r="T20" s="42"/>
+      <c r="U20" s="43"/>
     </row>
     <row r="21" spans="1:21">
-      <c r="A21" s="40"/>
-      <c r="B21" s="41"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="41"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="40"/>
-      <c r="I21" s="41"/>
-      <c r="J21" s="41"/>
-      <c r="K21" s="41"/>
-      <c r="L21" s="41"/>
-      <c r="M21" s="41"/>
-      <c r="N21" s="42"/>
-      <c r="O21" s="40"/>
-      <c r="P21" s="41"/>
-      <c r="Q21" s="41"/>
-      <c r="R21" s="41"/>
-      <c r="S21" s="41"/>
-      <c r="T21" s="41"/>
-      <c r="U21" s="42"/>
+      <c r="A21" s="41"/>
+      <c r="B21" s="42"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="41"/>
+      <c r="I21" s="42"/>
+      <c r="J21" s="42"/>
+      <c r="K21" s="42"/>
+      <c r="L21" s="42"/>
+      <c r="M21" s="42"/>
+      <c r="N21" s="43"/>
+      <c r="O21" s="41"/>
+      <c r="P21" s="42"/>
+      <c r="Q21" s="42"/>
+      <c r="R21" s="42"/>
+      <c r="S21" s="42"/>
+      <c r="T21" s="42"/>
+      <c r="U21" s="43"/>
     </row>
     <row r="22" spans="1:21">
-      <c r="A22" s="43"/>
-      <c r="B22" s="44"/>
-      <c r="C22" s="44"/>
-      <c r="D22" s="44"/>
-      <c r="E22" s="44"/>
-      <c r="F22" s="44"/>
-      <c r="G22" s="45"/>
-      <c r="H22" s="43"/>
-      <c r="I22" s="44"/>
-      <c r="J22" s="44"/>
-      <c r="K22" s="44"/>
-      <c r="L22" s="44"/>
-      <c r="M22" s="44"/>
-      <c r="N22" s="45"/>
-      <c r="O22" s="43"/>
-      <c r="P22" s="44"/>
-      <c r="Q22" s="44"/>
-      <c r="R22" s="44"/>
-      <c r="S22" s="44"/>
-      <c r="T22" s="44"/>
-      <c r="U22" s="45"/>
+      <c r="A22" s="44"/>
+      <c r="B22" s="45"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="46"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="45"/>
+      <c r="J22" s="45"/>
+      <c r="K22" s="45"/>
+      <c r="L22" s="45"/>
+      <c r="M22" s="45"/>
+      <c r="N22" s="46"/>
+      <c r="O22" s="44"/>
+      <c r="P22" s="45"/>
+      <c r="Q22" s="45"/>
+      <c r="R22" s="45"/>
+      <c r="S22" s="45"/>
+      <c r="T22" s="45"/>
+      <c r="U22" s="46"/>
     </row>
     <row r="23" spans="1:21">
-      <c r="A23" s="46"/>
-      <c r="B23" s="46"/>
-      <c r="C23" s="46"/>
-      <c r="D23" s="46"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="46"/>
-      <c r="I23" s="46"/>
-      <c r="J23" s="46"/>
-      <c r="K23" s="46"/>
-      <c r="L23" s="46"/>
-      <c r="M23" s="46"/>
-      <c r="N23" s="46"/>
-      <c r="O23" s="46"/>
-      <c r="P23" s="46"/>
-      <c r="Q23" s="46"/>
-      <c r="R23" s="46"/>
-      <c r="S23" s="46"/>
-      <c r="T23" s="46"/>
-      <c r="U23" s="46"/>
+      <c r="A23" s="37"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="37"/>
+      <c r="K23" s="37"/>
+      <c r="L23" s="37"/>
+      <c r="M23" s="37"/>
+      <c r="N23" s="37"/>
+      <c r="O23" s="37"/>
+      <c r="P23" s="37"/>
+      <c r="Q23" s="37"/>
+      <c r="R23" s="37"/>
+      <c r="S23" s="37"/>
+      <c r="T23" s="37"/>
+      <c r="U23" s="37"/>
     </row>
     <row r="24" spans="1:21">
-      <c r="A24" s="37"/>
-      <c r="B24" s="38"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="37"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="38"/>
-      <c r="K24" s="38"/>
-      <c r="L24" s="38"/>
-      <c r="M24" s="38"/>
-      <c r="N24" s="39"/>
-      <c r="O24" s="37"/>
-      <c r="P24" s="38"/>
-      <c r="Q24" s="38"/>
-      <c r="R24" s="38"/>
-      <c r="S24" s="38"/>
-      <c r="T24" s="38"/>
-      <c r="U24" s="39"/>
+      <c r="A24" s="38"/>
+      <c r="B24" s="39"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="39"/>
+      <c r="J24" s="39"/>
+      <c r="K24" s="39"/>
+      <c r="L24" s="39"/>
+      <c r="M24" s="39"/>
+      <c r="N24" s="40"/>
+      <c r="O24" s="38"/>
+      <c r="P24" s="39"/>
+      <c r="Q24" s="39"/>
+      <c r="R24" s="39"/>
+      <c r="S24" s="39"/>
+      <c r="T24" s="39"/>
+      <c r="U24" s="40"/>
     </row>
     <row r="25" spans="1:21">
-      <c r="A25" s="40"/>
-      <c r="B25" s="41"/>
-      <c r="C25" s="41"/>
-      <c r="D25" s="41"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="41"/>
-      <c r="G25" s="42"/>
-      <c r="H25" s="40"/>
-      <c r="I25" s="41"/>
-      <c r="J25" s="41"/>
-      <c r="K25" s="41"/>
-      <c r="L25" s="41"/>
-      <c r="M25" s="41"/>
-      <c r="N25" s="42"/>
-      <c r="O25" s="40"/>
-      <c r="P25" s="41"/>
-      <c r="Q25" s="41"/>
-      <c r="R25" s="41"/>
-      <c r="S25" s="41"/>
-      <c r="T25" s="41"/>
-      <c r="U25" s="42"/>
+      <c r="A25" s="41"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="43"/>
+      <c r="H25" s="41"/>
+      <c r="I25" s="42"/>
+      <c r="J25" s="42"/>
+      <c r="K25" s="42"/>
+      <c r="L25" s="42"/>
+      <c r="M25" s="42"/>
+      <c r="N25" s="43"/>
+      <c r="O25" s="41"/>
+      <c r="P25" s="42"/>
+      <c r="Q25" s="42"/>
+      <c r="R25" s="42"/>
+      <c r="S25" s="42"/>
+      <c r="T25" s="42"/>
+      <c r="U25" s="43"/>
     </row>
     <row r="26" spans="1:21">
-      <c r="A26" s="40"/>
-      <c r="B26" s="41"/>
-      <c r="C26" s="41"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="41"/>
-      <c r="F26" s="41"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="40"/>
-      <c r="I26" s="41"/>
-      <c r="J26" s="41"/>
-      <c r="K26" s="41"/>
-      <c r="L26" s="41"/>
-      <c r="M26" s="41"/>
-      <c r="N26" s="42"/>
-      <c r="O26" s="40"/>
-      <c r="P26" s="41"/>
-      <c r="Q26" s="41"/>
-      <c r="R26" s="41"/>
-      <c r="S26" s="41"/>
-      <c r="T26" s="41"/>
-      <c r="U26" s="42"/>
+      <c r="A26" s="41"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="43"/>
+      <c r="H26" s="41"/>
+      <c r="I26" s="42"/>
+      <c r="J26" s="42"/>
+      <c r="K26" s="42"/>
+      <c r="L26" s="42"/>
+      <c r="M26" s="42"/>
+      <c r="N26" s="43"/>
+      <c r="O26" s="41"/>
+      <c r="P26" s="42"/>
+      <c r="Q26" s="42"/>
+      <c r="R26" s="42"/>
+      <c r="S26" s="42"/>
+      <c r="T26" s="42"/>
+      <c r="U26" s="43"/>
     </row>
     <row r="27" spans="1:21">
-      <c r="A27" s="40"/>
-      <c r="B27" s="41"/>
-      <c r="C27" s="41"/>
-      <c r="D27" s="41"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="41"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="40"/>
-      <c r="I27" s="41"/>
-      <c r="J27" s="41"/>
-      <c r="K27" s="41"/>
-      <c r="L27" s="41"/>
-      <c r="M27" s="41"/>
-      <c r="N27" s="42"/>
-      <c r="O27" s="40"/>
-      <c r="P27" s="41"/>
-      <c r="Q27" s="41"/>
-      <c r="R27" s="41"/>
-      <c r="S27" s="41"/>
-      <c r="T27" s="41"/>
-      <c r="U27" s="42"/>
+      <c r="A27" s="41"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="43"/>
+      <c r="H27" s="41"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
+      <c r="K27" s="42"/>
+      <c r="L27" s="42"/>
+      <c r="M27" s="42"/>
+      <c r="N27" s="43"/>
+      <c r="O27" s="41"/>
+      <c r="P27" s="42"/>
+      <c r="Q27" s="42"/>
+      <c r="R27" s="42"/>
+      <c r="S27" s="42"/>
+      <c r="T27" s="42"/>
+      <c r="U27" s="43"/>
     </row>
     <row r="28" spans="1:21">
-      <c r="A28" s="40"/>
-      <c r="B28" s="41"/>
-      <c r="C28" s="41"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
-      <c r="G28" s="42"/>
-      <c r="H28" s="40"/>
-      <c r="I28" s="41"/>
-      <c r="J28" s="41"/>
-      <c r="K28" s="41"/>
-      <c r="L28" s="41"/>
-      <c r="M28" s="41"/>
-      <c r="N28" s="42"/>
-      <c r="O28" s="40"/>
-      <c r="P28" s="41"/>
-      <c r="Q28" s="41"/>
-      <c r="R28" s="41"/>
-      <c r="S28" s="41"/>
-      <c r="T28" s="41"/>
-      <c r="U28" s="42"/>
+      <c r="A28" s="41"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="42"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="41"/>
+      <c r="I28" s="42"/>
+      <c r="J28" s="42"/>
+      <c r="K28" s="42"/>
+      <c r="L28" s="42"/>
+      <c r="M28" s="42"/>
+      <c r="N28" s="43"/>
+      <c r="O28" s="41"/>
+      <c r="P28" s="42"/>
+      <c r="Q28" s="42"/>
+      <c r="R28" s="42"/>
+      <c r="S28" s="42"/>
+      <c r="T28" s="42"/>
+      <c r="U28" s="43"/>
     </row>
     <row r="29" spans="1:21">
-      <c r="A29" s="40"/>
-      <c r="B29" s="41"/>
-      <c r="C29" s="41"/>
-      <c r="D29" s="41"/>
-      <c r="E29" s="41"/>
-      <c r="F29" s="41"/>
-      <c r="G29" s="42"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="41"/>
-      <c r="J29" s="41"/>
-      <c r="K29" s="41"/>
-      <c r="L29" s="41"/>
-      <c r="M29" s="41"/>
-      <c r="N29" s="42"/>
-      <c r="O29" s="40"/>
-      <c r="P29" s="41"/>
-      <c r="Q29" s="41"/>
-      <c r="R29" s="41"/>
-      <c r="S29" s="41"/>
-      <c r="T29" s="41"/>
-      <c r="U29" s="42"/>
+      <c r="A29" s="41"/>
+      <c r="B29" s="42"/>
+      <c r="C29" s="42"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="41"/>
+      <c r="I29" s="42"/>
+      <c r="J29" s="42"/>
+      <c r="K29" s="42"/>
+      <c r="L29" s="42"/>
+      <c r="M29" s="42"/>
+      <c r="N29" s="43"/>
+      <c r="O29" s="41"/>
+      <c r="P29" s="42"/>
+      <c r="Q29" s="42"/>
+      <c r="R29" s="42"/>
+      <c r="S29" s="42"/>
+      <c r="T29" s="42"/>
+      <c r="U29" s="43"/>
     </row>
     <row r="30" spans="1:21">
-      <c r="A30" s="40"/>
-      <c r="B30" s="41"/>
-      <c r="C30" s="41"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="41"/>
-      <c r="F30" s="41"/>
-      <c r="G30" s="42"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="41"/>
-      <c r="J30" s="41"/>
-      <c r="K30" s="41"/>
-      <c r="L30" s="41"/>
-      <c r="M30" s="41"/>
-      <c r="N30" s="42"/>
-      <c r="O30" s="40"/>
-      <c r="P30" s="41"/>
-      <c r="Q30" s="41"/>
-      <c r="R30" s="41"/>
-      <c r="S30" s="41"/>
-      <c r="T30" s="41"/>
-      <c r="U30" s="42"/>
+      <c r="A30" s="41"/>
+      <c r="B30" s="42"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="41"/>
+      <c r="I30" s="42"/>
+      <c r="J30" s="42"/>
+      <c r="K30" s="42"/>
+      <c r="L30" s="42"/>
+      <c r="M30" s="42"/>
+      <c r="N30" s="43"/>
+      <c r="O30" s="41"/>
+      <c r="P30" s="42"/>
+      <c r="Q30" s="42"/>
+      <c r="R30" s="42"/>
+      <c r="S30" s="42"/>
+      <c r="T30" s="42"/>
+      <c r="U30" s="43"/>
     </row>
     <row r="31" spans="1:21">
-      <c r="A31" s="40"/>
-      <c r="B31" s="41"/>
-      <c r="C31" s="41"/>
-      <c r="D31" s="41"/>
-      <c r="E31" s="41"/>
-      <c r="F31" s="41"/>
-      <c r="G31" s="42"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="41"/>
-      <c r="J31" s="41"/>
-      <c r="K31" s="41"/>
-      <c r="L31" s="41"/>
-      <c r="M31" s="41"/>
-      <c r="N31" s="42"/>
-      <c r="O31" s="40"/>
-      <c r="P31" s="41"/>
-      <c r="Q31" s="41"/>
-      <c r="R31" s="41"/>
-      <c r="S31" s="41"/>
-      <c r="T31" s="41"/>
-      <c r="U31" s="42"/>
+      <c r="A31" s="41"/>
+      <c r="B31" s="42"/>
+      <c r="C31" s="42"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="43"/>
+      <c r="H31" s="41"/>
+      <c r="I31" s="42"/>
+      <c r="J31" s="42"/>
+      <c r="K31" s="42"/>
+      <c r="L31" s="42"/>
+      <c r="M31" s="42"/>
+      <c r="N31" s="43"/>
+      <c r="O31" s="41"/>
+      <c r="P31" s="42"/>
+      <c r="Q31" s="42"/>
+      <c r="R31" s="42"/>
+      <c r="S31" s="42"/>
+      <c r="T31" s="42"/>
+      <c r="U31" s="43"/>
     </row>
     <row r="32" spans="1:21">
-      <c r="A32" s="40"/>
-      <c r="B32" s="41"/>
-      <c r="C32" s="41"/>
-      <c r="D32" s="41"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="41"/>
-      <c r="G32" s="42"/>
-      <c r="H32" s="40"/>
-      <c r="I32" s="41"/>
-      <c r="J32" s="41"/>
-      <c r="K32" s="41"/>
-      <c r="L32" s="41"/>
-      <c r="M32" s="41"/>
-      <c r="N32" s="42"/>
-      <c r="O32" s="40"/>
-      <c r="P32" s="41"/>
-      <c r="Q32" s="41"/>
-      <c r="R32" s="41"/>
-      <c r="S32" s="41"/>
-      <c r="T32" s="41"/>
-      <c r="U32" s="42"/>
+      <c r="A32" s="41"/>
+      <c r="B32" s="42"/>
+      <c r="C32" s="42"/>
+      <c r="D32" s="42"/>
+      <c r="E32" s="42"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="43"/>
+      <c r="H32" s="41"/>
+      <c r="I32" s="42"/>
+      <c r="J32" s="42"/>
+      <c r="K32" s="42"/>
+      <c r="L32" s="42"/>
+      <c r="M32" s="42"/>
+      <c r="N32" s="43"/>
+      <c r="O32" s="41"/>
+      <c r="P32" s="42"/>
+      <c r="Q32" s="42"/>
+      <c r="R32" s="42"/>
+      <c r="S32" s="42"/>
+      <c r="T32" s="42"/>
+      <c r="U32" s="43"/>
     </row>
     <row r="33" spans="1:21">
-      <c r="A33" s="43"/>
-      <c r="B33" s="44"/>
-      <c r="C33" s="44"/>
-      <c r="D33" s="44"/>
-      <c r="E33" s="44"/>
-      <c r="F33" s="44"/>
-      <c r="G33" s="45"/>
-      <c r="H33" s="43"/>
-      <c r="I33" s="44"/>
-      <c r="J33" s="44"/>
-      <c r="K33" s="44"/>
-      <c r="L33" s="44"/>
-      <c r="M33" s="44"/>
-      <c r="N33" s="45"/>
-      <c r="O33" s="43"/>
-      <c r="P33" s="44"/>
-      <c r="Q33" s="44"/>
-      <c r="R33" s="44"/>
-      <c r="S33" s="44"/>
-      <c r="T33" s="44"/>
-      <c r="U33" s="45"/>
+      <c r="A33" s="44"/>
+      <c r="B33" s="45"/>
+      <c r="C33" s="45"/>
+      <c r="D33" s="45"/>
+      <c r="E33" s="45"/>
+      <c r="F33" s="45"/>
+      <c r="G33" s="46"/>
+      <c r="H33" s="44"/>
+      <c r="I33" s="45"/>
+      <c r="J33" s="45"/>
+      <c r="K33" s="45"/>
+      <c r="L33" s="45"/>
+      <c r="M33" s="45"/>
+      <c r="N33" s="46"/>
+      <c r="O33" s="44"/>
+      <c r="P33" s="45"/>
+      <c r="Q33" s="45"/>
+      <c r="R33" s="45"/>
+      <c r="S33" s="45"/>
+      <c r="T33" s="45"/>
+      <c r="U33" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A24:G33"/>
+    <mergeCell ref="H23:N23"/>
+    <mergeCell ref="H24:N33"/>
+    <mergeCell ref="O23:U23"/>
+    <mergeCell ref="O24:U33"/>
     <mergeCell ref="O1:U1"/>
     <mergeCell ref="O2:U11"/>
     <mergeCell ref="O12:U12"/>
     <mergeCell ref="O13:U22"/>
     <mergeCell ref="A23:G23"/>
-    <mergeCell ref="A24:G33"/>
-    <mergeCell ref="H23:N23"/>
-    <mergeCell ref="H24:N33"/>
-    <mergeCell ref="O23:U23"/>
-    <mergeCell ref="O24:U33"/>
     <mergeCell ref="A2:G11"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="H1:N1"/>

</xml_diff>

<commit_message>
revising UART2 and system design
</commit_message>
<xml_diff>
--- a/SecSys_TM4C/SecSys.xlsx
+++ b/SecSys_TM4C/SecSys.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="PIn Map" sheetId="1" r:id="rId1"/>
+    <sheet name="Pin Map" sheetId="1" r:id="rId1"/>
     <sheet name="TODO" sheetId="2" r:id="rId2"/>
     <sheet name="Timer Reload Value" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
+    <sheet name="OS Tasks" sheetId="4" r:id="rId4"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'OS Tasks'!$A$1:$E$24</definedName>
     <definedName name="R_1">'[1]Light sensor #1'!$D$1</definedName>
     <definedName name="R_2">'[1]Light sensor #1'!$D$2</definedName>
     <definedName name="R_3">'[1]Light sensor #1'!$D$3</definedName>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="159">
   <si>
     <t>Port / Pin</t>
   </si>
@@ -501,6 +502,174 @@
       <t>=7,999.</t>
     </r>
   </si>
+  <si>
+    <t>PIR A, edge trigered PC6</t>
+  </si>
+  <si>
+    <t>PIR B, edge trigered PC7</t>
+  </si>
+  <si>
+    <t>Function &amp; Type</t>
+  </si>
+  <si>
+    <t>Wait for…</t>
+  </si>
+  <si>
+    <t>SemPortC.pin6</t>
+  </si>
+  <si>
+    <t>SemPortC.pin7</t>
+  </si>
+  <si>
+    <t>Task7Sync</t>
+  </si>
+  <si>
+    <t>Task8Sync</t>
+  </si>
+  <si>
+    <t>Task Nr.</t>
+  </si>
+  <si>
+    <t>PerTask[0].semaphore</t>
+  </si>
+  <si>
+    <t>Signal or Call func.</t>
+  </si>
+  <si>
+    <t>CYCL_10ms()</t>
+  </si>
+  <si>
+    <t>PerTask[1].semaphore</t>
+  </si>
+  <si>
+    <t>CYCL_50ms()</t>
+  </si>
+  <si>
+    <t>PerTask[2].semaphore</t>
+  </si>
+  <si>
+    <t>CYCL_100ms()</t>
+  </si>
+  <si>
+    <t>Cyclic 500 ms</t>
+  </si>
+  <si>
+    <t>Cyclic 100 ms</t>
+  </si>
+  <si>
+    <t>Cyclic 50 ms</t>
+  </si>
+  <si>
+    <t>Cyclic 10 ms</t>
+  </si>
+  <si>
+    <t>CYCL_500ms()</t>
+  </si>
+  <si>
+    <t>PerTask[3].semaphore</t>
+  </si>
+  <si>
+    <t>PerTask[4].semaphore</t>
+  </si>
+  <si>
+    <t>Cyclic 1000 ms</t>
+  </si>
+  <si>
+    <t>CYCL_1000ms()</t>
+  </si>
+  <si>
+    <t>Task 0</t>
+  </si>
+  <si>
+    <t>Task 1</t>
+  </si>
+  <si>
+    <t>Task 2</t>
+  </si>
+  <si>
+    <t>Task 3</t>
+  </si>
+  <si>
+    <t>Task 4</t>
+  </si>
+  <si>
+    <t>Task 5</t>
+  </si>
+  <si>
+    <t>Task 6</t>
+  </si>
+  <si>
+    <t>Task 7</t>
+  </si>
+  <si>
+    <t>Task 8</t>
+  </si>
+  <si>
+    <t>Task 9</t>
+  </si>
+  <si>
+    <t>Task 10</t>
+  </si>
+  <si>
+    <t>Task 11</t>
+  </si>
+  <si>
+    <t>Task 12</t>
+  </si>
+  <si>
+    <t>Task 13</t>
+  </si>
+  <si>
+    <t>Task 14</t>
+  </si>
+  <si>
+    <t>Task 15</t>
+  </si>
+  <si>
+    <t>Task 16</t>
+  </si>
+  <si>
+    <t>Task 17</t>
+  </si>
+  <si>
+    <t>Task 18</t>
+  </si>
+  <si>
+    <t>Task 19</t>
+  </si>
+  <si>
+    <t>Task 20</t>
+  </si>
+  <si>
+    <t>Task 21</t>
+  </si>
+  <si>
+    <t>Process PIR A</t>
+  </si>
+  <si>
+    <t>Process PIR B</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Idle Task</t>
+  </si>
+  <si>
+    <t>Never sleeps, never waits, just idle</t>
+  </si>
+  <si>
+    <t>Blank Task - Send SMS, edge trigered PF0</t>
+  </si>
+  <si>
+    <t>Blank Task - Receive SMS, edge trigered PF4</t>
+  </si>
+  <si>
+    <t>SemPortF.pin0</t>
+  </si>
+  <si>
+    <t>SemPortF.pin4</t>
+  </si>
 </sst>
 </file>
 
@@ -509,7 +678,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -599,8 +768,15 @@
       <family val="2"/>
       <charset val="238"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="22">
+  <fills count="24">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -727,6 +903,18 @@
         <bgColor rgb="FFDDDDDD"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -793,26 +981,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -853,6 +1023,27 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -1255,8 +1446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1272,615 +1463,615 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="3.75" customHeight="1">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="6"/>
-      <c r="B4" s="10" t="s">
+      <c r="A4" s="34"/>
+      <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="6"/>
-      <c r="B5" s="10" t="s">
+      <c r="A5" s="34"/>
+      <c r="B5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="6"/>
-      <c r="B6" s="10" t="s">
+      <c r="A6" s="34"/>
+      <c r="B6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="6"/>
-      <c r="B7" s="10" t="s">
+      <c r="A7" s="34"/>
+      <c r="B7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="11"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="6"/>
-      <c r="B8" s="10" t="s">
+      <c r="A8" s="34"/>
+      <c r="B8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="6"/>
-      <c r="B9" s="10" t="s">
+      <c r="A9" s="34"/>
+      <c r="B9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="6"/>
-      <c r="B10" s="10" t="s">
+      <c r="A10" s="34"/>
+      <c r="B10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:7" ht="3.75" customHeight="1">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="6"/>
-      <c r="B13" s="10" t="s">
+      <c r="A13" s="34"/>
+      <c r="B13" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="6"/>
-      <c r="B14" s="10" t="s">
+      <c r="A14" s="34"/>
+      <c r="B14" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="6"/>
-      <c r="B15" s="10" t="s">
+      <c r="A15" s="34"/>
+      <c r="B15" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="6"/>
-      <c r="B16" s="10" t="s">
+      <c r="A16" s="34"/>
+      <c r="B16" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="6"/>
-      <c r="B17" s="10" t="s">
+      <c r="A17" s="34"/>
+      <c r="B17" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="6"/>
-      <c r="B18" s="10" t="s">
+      <c r="A18" s="34"/>
+      <c r="B18" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:7" ht="3.75" customHeight="1">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="35"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="6"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
+      <c r="A21" s="34"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="35"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="6"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
+      <c r="A22" s="34"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="35"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="6"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
+      <c r="A23" s="34"/>
+      <c r="B23" s="35"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="35"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="6"/>
-      <c r="B24" s="14" t="s">
+      <c r="A24" s="34"/>
+      <c r="B24" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="6"/>
-      <c r="B25" s="14" t="s">
+      <c r="A25" s="34"/>
+      <c r="B25" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="6"/>
-      <c r="B26" s="14" t="s">
+      <c r="A26" s="34"/>
+      <c r="B26" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="D26" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E26" s="14" t="s">
+      <c r="E26" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="F26" s="14" t="s">
+      <c r="F26" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G26" s="10" t="s">
+      <c r="G26" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="6"/>
-      <c r="B27" s="14" t="s">
+      <c r="A27" s="34"/>
+      <c r="B27" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="F27" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G27" s="10" t="s">
+      <c r="G27" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="3.75" customHeight="1">
-      <c r="A28" s="9"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="6"/>
-      <c r="B30" s="11" t="s">
+      <c r="A30" s="34"/>
+      <c r="B30" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="6"/>
-      <c r="B31" s="11" t="s">
+      <c r="A31" s="34"/>
+      <c r="B31" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="6"/>
-      <c r="B32" s="11" t="s">
+      <c r="A32" s="34"/>
+      <c r="B32" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="6"/>
-      <c r="B33" s="15" t="s">
+      <c r="A33" s="34"/>
+      <c r="B33" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D33" s="11" t="s">
+      <c r="D33" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E33" s="10" t="s">
+      <c r="E33" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F33" s="10" t="s">
+      <c r="F33" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G33" s="10" t="s">
+      <c r="G33" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="6"/>
-      <c r="B34" s="10" t="s">
+      <c r="A34" s="34"/>
+      <c r="B34" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D34" s="11" t="s">
+      <c r="D34" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E34" s="10" t="s">
+      <c r="E34" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F34" s="10" t="s">
+      <c r="F34" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G34" s="10" t="s">
+      <c r="G34" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="3.75" customHeight="1">
-      <c r="A35" s="9"/>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
     </row>
     <row r="36" spans="1:7" ht="15" customHeight="1">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="B36" s="15" t="s">
+      <c r="B36" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
     </row>
     <row r="37" spans="1:7" ht="15" customHeight="1">
-      <c r="A37" s="4"/>
-      <c r="B37" s="10" t="s">
+      <c r="A37" s="33"/>
+      <c r="B37" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C37" s="14" t="s">
+      <c r="C37" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D37" s="11"/>
-      <c r="E37" s="10" t="s">
+      <c r="D37" s="5"/>
+      <c r="E37" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
     </row>
     <row r="38" spans="1:7" ht="15" customHeight="1">
-      <c r="A38" s="4"/>
-      <c r="B38" s="10" t="s">
+      <c r="A38" s="33"/>
+      <c r="B38" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C38" s="14" t="s">
+      <c r="C38" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10" t="s">
+      <c r="D38" s="4"/>
+      <c r="E38" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
     </row>
     <row r="39" spans="1:7" ht="15" customHeight="1">
-      <c r="A39" s="4"/>
-      <c r="B39" s="10" t="s">
+      <c r="A39" s="33"/>
+      <c r="B39" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C39" s="14" t="s">
+      <c r="C39" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D39" s="10"/>
-      <c r="E39" s="10" t="s">
+      <c r="D39" s="4"/>
+      <c r="E39" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="4"/>
-      <c r="B40" s="10" t="s">
+      <c r="A40" s="33"/>
+      <c r="B40" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C40" s="13"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="4"/>
-      <c r="B41" s="10" t="s">
+      <c r="A41" s="33"/>
+      <c r="B41" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C41" s="13"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="10"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
     </row>
     <row r="42" spans="1:7" ht="3.75" customHeight="1">
-      <c r="A42" s="9"/>
-      <c r="B42" s="9"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9"/>
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="6" t="s">
+      <c r="A43" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="B43" s="10" t="s">
+      <c r="B43" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="10"/>
-      <c r="G43" s="10"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="6"/>
-      <c r="B44" s="12" t="s">
+      <c r="A44" s="34"/>
+      <c r="B44" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C44" s="10"/>
-      <c r="D44" s="10"/>
-      <c r="E44" s="10"/>
-      <c r="F44" s="10"/>
-      <c r="G44" s="10"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="6"/>
-      <c r="B45" s="16" t="s">
+      <c r="A45" s="34"/>
+      <c r="B45" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="C45" s="10"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="10"/>
-      <c r="F45" s="10"/>
-      <c r="G45" s="10"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="6"/>
-      <c r="B46" s="17" t="s">
+      <c r="A46" s="34"/>
+      <c r="B46" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="C46" s="10"/>
-      <c r="D46" s="10"/>
-      <c r="E46" s="10"/>
-      <c r="F46" s="10"/>
-      <c r="G46" s="10"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="6"/>
-      <c r="B47" s="10" t="s">
+      <c r="A47" s="34"/>
+      <c r="B47" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C47" s="10"/>
-      <c r="D47" s="10"/>
-      <c r="E47" s="10"/>
-      <c r="F47" s="10"/>
-      <c r="G47" s="10"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
     </row>
     <row r="48" spans="1:7" ht="3.75" customHeight="1">
-      <c r="A48" s="9"/>
-      <c r="B48" s="9"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="9"/>
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="B20:G23"/>
+    <mergeCell ref="A29:A34"/>
     <mergeCell ref="A36:A41"/>
     <mergeCell ref="A43:A47"/>
     <mergeCell ref="A3:A10"/>
     <mergeCell ref="A12:A18"/>
     <mergeCell ref="A20:A27"/>
-    <mergeCell ref="B20:G23"/>
-    <mergeCell ref="A29:A34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1892,7 +2083,7 @@
   <dimension ref="A1:U33"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+      <selection activeCell="O23" sqref="O23:U23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1901,802 +2092,802 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3" t="s">
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="36"/>
     </row>
     <row r="2" spans="1:21" ht="15" customHeight="1">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="1" t="s">
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="37"/>
     </row>
     <row r="3" spans="1:21">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
+      <c r="A3" s="37"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="37"/>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="37"/>
+      <c r="R3" s="37"/>
+      <c r="S3" s="37"/>
+      <c r="T3" s="37"/>
+      <c r="U3" s="37"/>
     </row>
     <row r="4" spans="1:21">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
+      <c r="A4" s="37"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="38"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="38"/>
+      <c r="N4" s="38"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="37"/>
+      <c r="Q4" s="37"/>
+      <c r="R4" s="37"/>
+      <c r="S4" s="37"/>
+      <c r="T4" s="37"/>
+      <c r="U4" s="37"/>
     </row>
     <row r="5" spans="1:21">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
+      <c r="A5" s="37"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="38"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="38"/>
+      <c r="N5" s="38"/>
+      <c r="O5" s="37"/>
+      <c r="P5" s="37"/>
+      <c r="Q5" s="37"/>
+      <c r="R5" s="37"/>
+      <c r="S5" s="37"/>
+      <c r="T5" s="37"/>
+      <c r="U5" s="37"/>
     </row>
     <row r="6" spans="1:21">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
-      <c r="U6" s="2"/>
+      <c r="A6" s="37"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="38"/>
+      <c r="L6" s="38"/>
+      <c r="M6" s="38"/>
+      <c r="N6" s="38"/>
+      <c r="O6" s="37"/>
+      <c r="P6" s="37"/>
+      <c r="Q6" s="37"/>
+      <c r="R6" s="37"/>
+      <c r="S6" s="37"/>
+      <c r="T6" s="37"/>
+      <c r="U6" s="37"/>
     </row>
     <row r="7" spans="1:21">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
+      <c r="A7" s="37"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="38"/>
+      <c r="N7" s="38"/>
+      <c r="O7" s="37"/>
+      <c r="P7" s="37"/>
+      <c r="Q7" s="37"/>
+      <c r="R7" s="37"/>
+      <c r="S7" s="37"/>
+      <c r="T7" s="37"/>
+      <c r="U7" s="37"/>
     </row>
     <row r="8" spans="1:21">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
-      <c r="U8" s="2"/>
+      <c r="A8" s="37"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="38"/>
+      <c r="M8" s="38"/>
+      <c r="N8" s="38"/>
+      <c r="O8" s="37"/>
+      <c r="P8" s="37"/>
+      <c r="Q8" s="37"/>
+      <c r="R8" s="37"/>
+      <c r="S8" s="37"/>
+      <c r="T8" s="37"/>
+      <c r="U8" s="37"/>
     </row>
     <row r="9" spans="1:21">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
-      <c r="U9" s="2"/>
+      <c r="A9" s="37"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="38"/>
+      <c r="L9" s="38"/>
+      <c r="M9" s="38"/>
+      <c r="N9" s="38"/>
+      <c r="O9" s="37"/>
+      <c r="P9" s="37"/>
+      <c r="Q9" s="37"/>
+      <c r="R9" s="37"/>
+      <c r="S9" s="37"/>
+      <c r="T9" s="37"/>
+      <c r="U9" s="37"/>
     </row>
     <row r="10" spans="1:21">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="2"/>
-      <c r="U10" s="2"/>
+      <c r="A10" s="37"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="38"/>
+      <c r="M10" s="38"/>
+      <c r="N10" s="38"/>
+      <c r="O10" s="37"/>
+      <c r="P10" s="37"/>
+      <c r="Q10" s="37"/>
+      <c r="R10" s="37"/>
+      <c r="S10" s="37"/>
+      <c r="T10" s="37"/>
+      <c r="U10" s="37"/>
     </row>
     <row r="11" spans="1:21">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
-      <c r="T11" s="2"/>
-      <c r="U11" s="2"/>
+      <c r="A11" s="37"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="38"/>
+      <c r="L11" s="38"/>
+      <c r="M11" s="38"/>
+      <c r="N11" s="38"/>
+      <c r="O11" s="37"/>
+      <c r="P11" s="37"/>
+      <c r="Q11" s="37"/>
+      <c r="R11" s="37"/>
+      <c r="S11" s="37"/>
+      <c r="T11" s="37"/>
+      <c r="U11" s="37"/>
     </row>
     <row r="12" spans="1:21">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3" t="s">
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="3"/>
-      <c r="S12" s="3"/>
-      <c r="T12" s="3"/>
-      <c r="U12" s="3"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="36"/>
+      <c r="K12" s="36"/>
+      <c r="L12" s="36"/>
+      <c r="M12" s="36"/>
+      <c r="N12" s="36"/>
+      <c r="O12" s="36"/>
+      <c r="P12" s="36"/>
+      <c r="Q12" s="36"/>
+      <c r="R12" s="36"/>
+      <c r="S12" s="36"/>
+      <c r="T12" s="36"/>
+      <c r="U12" s="36"/>
     </row>
     <row r="13" spans="1:21" ht="15" customHeight="1">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2" t="s">
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="2"/>
-      <c r="S13" s="2"/>
-      <c r="T13" s="2"/>
-      <c r="U13" s="2"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="37"/>
+      <c r="M13" s="37"/>
+      <c r="N13" s="37"/>
+      <c r="O13" s="37"/>
+      <c r="P13" s="37"/>
+      <c r="Q13" s="37"/>
+      <c r="R13" s="37"/>
+      <c r="S13" s="37"/>
+      <c r="T13" s="37"/>
+      <c r="U13" s="37"/>
     </row>
     <row r="14" spans="1:21">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="2"/>
-      <c r="R14" s="2"/>
-      <c r="S14" s="2"/>
-      <c r="T14" s="2"/>
-      <c r="U14" s="2"/>
+      <c r="A14" s="37"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="37"/>
+      <c r="M14" s="37"/>
+      <c r="N14" s="37"/>
+      <c r="O14" s="37"/>
+      <c r="P14" s="37"/>
+      <c r="Q14" s="37"/>
+      <c r="R14" s="37"/>
+      <c r="S14" s="37"/>
+      <c r="T14" s="37"/>
+      <c r="U14" s="37"/>
     </row>
     <row r="15" spans="1:21">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="2"/>
-      <c r="S15" s="2"/>
-      <c r="T15" s="2"/>
-      <c r="U15" s="2"/>
+      <c r="A15" s="37"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="37"/>
+      <c r="L15" s="37"/>
+      <c r="M15" s="37"/>
+      <c r="N15" s="37"/>
+      <c r="O15" s="37"/>
+      <c r="P15" s="37"/>
+      <c r="Q15" s="37"/>
+      <c r="R15" s="37"/>
+      <c r="S15" s="37"/>
+      <c r="T15" s="37"/>
+      <c r="U15" s="37"/>
     </row>
     <row r="16" spans="1:21">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2"/>
-      <c r="R16" s="2"/>
-      <c r="S16" s="2"/>
-      <c r="T16" s="2"/>
-      <c r="U16" s="2"/>
+      <c r="A16" s="37"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="37"/>
+      <c r="L16" s="37"/>
+      <c r="M16" s="37"/>
+      <c r="N16" s="37"/>
+      <c r="O16" s="37"/>
+      <c r="P16" s="37"/>
+      <c r="Q16" s="37"/>
+      <c r="R16" s="37"/>
+      <c r="S16" s="37"/>
+      <c r="T16" s="37"/>
+      <c r="U16" s="37"/>
     </row>
     <row r="17" spans="1:21">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
-      <c r="Q17" s="2"/>
-      <c r="R17" s="2"/>
-      <c r="S17" s="2"/>
-      <c r="T17" s="2"/>
-      <c r="U17" s="2"/>
+      <c r="A17" s="37"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="37"/>
+      <c r="L17" s="37"/>
+      <c r="M17" s="37"/>
+      <c r="N17" s="37"/>
+      <c r="O17" s="37"/>
+      <c r="P17" s="37"/>
+      <c r="Q17" s="37"/>
+      <c r="R17" s="37"/>
+      <c r="S17" s="37"/>
+      <c r="T17" s="37"/>
+      <c r="U17" s="37"/>
     </row>
     <row r="18" spans="1:21">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="2"/>
-      <c r="R18" s="2"/>
-      <c r="S18" s="2"/>
-      <c r="T18" s="2"/>
-      <c r="U18" s="2"/>
+      <c r="A18" s="37"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="37"/>
+      <c r="L18" s="37"/>
+      <c r="M18" s="37"/>
+      <c r="N18" s="37"/>
+      <c r="O18" s="37"/>
+      <c r="P18" s="37"/>
+      <c r="Q18" s="37"/>
+      <c r="R18" s="37"/>
+      <c r="S18" s="37"/>
+      <c r="T18" s="37"/>
+      <c r="U18" s="37"/>
     </row>
     <row r="19" spans="1:21">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
-      <c r="Q19" s="2"/>
-      <c r="R19" s="2"/>
-      <c r="S19" s="2"/>
-      <c r="T19" s="2"/>
-      <c r="U19" s="2"/>
+      <c r="A19" s="37"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
+      <c r="K19" s="37"/>
+      <c r="L19" s="37"/>
+      <c r="M19" s="37"/>
+      <c r="N19" s="37"/>
+      <c r="O19" s="37"/>
+      <c r="P19" s="37"/>
+      <c r="Q19" s="37"/>
+      <c r="R19" s="37"/>
+      <c r="S19" s="37"/>
+      <c r="T19" s="37"/>
+      <c r="U19" s="37"/>
     </row>
     <row r="20" spans="1:21">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
-      <c r="Q20" s="2"/>
-      <c r="R20" s="2"/>
-      <c r="S20" s="2"/>
-      <c r="T20" s="2"/>
-      <c r="U20" s="2"/>
+      <c r="A20" s="37"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="37"/>
+      <c r="L20" s="37"/>
+      <c r="M20" s="37"/>
+      <c r="N20" s="37"/>
+      <c r="O20" s="37"/>
+      <c r="P20" s="37"/>
+      <c r="Q20" s="37"/>
+      <c r="R20" s="37"/>
+      <c r="S20" s="37"/>
+      <c r="T20" s="37"/>
+      <c r="U20" s="37"/>
     </row>
     <row r="21" spans="1:21">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
-      <c r="P21" s="2"/>
-      <c r="Q21" s="2"/>
-      <c r="R21" s="2"/>
-      <c r="S21" s="2"/>
-      <c r="T21" s="2"/>
-      <c r="U21" s="2"/>
+      <c r="A21" s="37"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="37"/>
+      <c r="L21" s="37"/>
+      <c r="M21" s="37"/>
+      <c r="N21" s="37"/>
+      <c r="O21" s="37"/>
+      <c r="P21" s="37"/>
+      <c r="Q21" s="37"/>
+      <c r="R21" s="37"/>
+      <c r="S21" s="37"/>
+      <c r="T21" s="37"/>
+      <c r="U21" s="37"/>
     </row>
     <row r="22" spans="1:21">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
-      <c r="P22" s="2"/>
-      <c r="Q22" s="2"/>
-      <c r="R22" s="2"/>
-      <c r="S22" s="2"/>
-      <c r="T22" s="2"/>
-      <c r="U22" s="2"/>
+      <c r="A22" s="37"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="37"/>
+      <c r="L22" s="37"/>
+      <c r="M22" s="37"/>
+      <c r="N22" s="37"/>
+      <c r="O22" s="37"/>
+      <c r="P22" s="37"/>
+      <c r="Q22" s="37"/>
+      <c r="R22" s="37"/>
+      <c r="S22" s="37"/>
+      <c r="T22" s="37"/>
+      <c r="U22" s="37"/>
     </row>
     <row r="23" spans="1:21">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="3"/>
-      <c r="R23" s="3"/>
-      <c r="S23" s="3"/>
-      <c r="T23" s="3"/>
-      <c r="U23" s="3"/>
+      <c r="A23" s="36"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="36"/>
+      <c r="J23" s="36"/>
+      <c r="K23" s="36"/>
+      <c r="L23" s="36"/>
+      <c r="M23" s="36"/>
+      <c r="N23" s="36"/>
+      <c r="O23" s="36"/>
+      <c r="P23" s="36"/>
+      <c r="Q23" s="36"/>
+      <c r="R23" s="36"/>
+      <c r="S23" s="36"/>
+      <c r="T23" s="36"/>
+      <c r="U23" s="36"/>
     </row>
     <row r="24" spans="1:21">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
-      <c r="O24" s="2"/>
-      <c r="P24" s="2"/>
-      <c r="Q24" s="2"/>
-      <c r="R24" s="2"/>
-      <c r="S24" s="2"/>
-      <c r="T24" s="2"/>
-      <c r="U24" s="2"/>
+      <c r="A24" s="37"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="37"/>
+      <c r="J24" s="37"/>
+      <c r="K24" s="37"/>
+      <c r="L24" s="37"/>
+      <c r="M24" s="37"/>
+      <c r="N24" s="37"/>
+      <c r="O24" s="37"/>
+      <c r="P24" s="37"/>
+      <c r="Q24" s="37"/>
+      <c r="R24" s="37"/>
+      <c r="S24" s="37"/>
+      <c r="T24" s="37"/>
+      <c r="U24" s="37"/>
     </row>
     <row r="25" spans="1:21">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
-      <c r="O25" s="2"/>
-      <c r="P25" s="2"/>
-      <c r="Q25" s="2"/>
-      <c r="R25" s="2"/>
-      <c r="S25" s="2"/>
-      <c r="T25" s="2"/>
-      <c r="U25" s="2"/>
+      <c r="A25" s="37"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="37"/>
+      <c r="K25" s="37"/>
+      <c r="L25" s="37"/>
+      <c r="M25" s="37"/>
+      <c r="N25" s="37"/>
+      <c r="O25" s="37"/>
+      <c r="P25" s="37"/>
+      <c r="Q25" s="37"/>
+      <c r="R25" s="37"/>
+      <c r="S25" s="37"/>
+      <c r="T25" s="37"/>
+      <c r="U25" s="37"/>
     </row>
     <row r="26" spans="1:21">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
-      <c r="O26" s="2"/>
-      <c r="P26" s="2"/>
-      <c r="Q26" s="2"/>
-      <c r="R26" s="2"/>
-      <c r="S26" s="2"/>
-      <c r="T26" s="2"/>
-      <c r="U26" s="2"/>
+      <c r="A26" s="37"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="37"/>
+      <c r="L26" s="37"/>
+      <c r="M26" s="37"/>
+      <c r="N26" s="37"/>
+      <c r="O26" s="37"/>
+      <c r="P26" s="37"/>
+      <c r="Q26" s="37"/>
+      <c r="R26" s="37"/>
+      <c r="S26" s="37"/>
+      <c r="T26" s="37"/>
+      <c r="U26" s="37"/>
     </row>
     <row r="27" spans="1:21">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
-      <c r="N27" s="2"/>
-      <c r="O27" s="2"/>
-      <c r="P27" s="2"/>
-      <c r="Q27" s="2"/>
-      <c r="R27" s="2"/>
-      <c r="S27" s="2"/>
-      <c r="T27" s="2"/>
-      <c r="U27" s="2"/>
+      <c r="A27" s="37"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
+      <c r="K27" s="37"/>
+      <c r="L27" s="37"/>
+      <c r="M27" s="37"/>
+      <c r="N27" s="37"/>
+      <c r="O27" s="37"/>
+      <c r="P27" s="37"/>
+      <c r="Q27" s="37"/>
+      <c r="R27" s="37"/>
+      <c r="S27" s="37"/>
+      <c r="T27" s="37"/>
+      <c r="U27" s="37"/>
     </row>
     <row r="28" spans="1:21">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
-      <c r="O28" s="2"/>
-      <c r="P28" s="2"/>
-      <c r="Q28" s="2"/>
-      <c r="R28" s="2"/>
-      <c r="S28" s="2"/>
-      <c r="T28" s="2"/>
-      <c r="U28" s="2"/>
+      <c r="A28" s="37"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
+      <c r="K28" s="37"/>
+      <c r="L28" s="37"/>
+      <c r="M28" s="37"/>
+      <c r="N28" s="37"/>
+      <c r="O28" s="37"/>
+      <c r="P28" s="37"/>
+      <c r="Q28" s="37"/>
+      <c r="R28" s="37"/>
+      <c r="S28" s="37"/>
+      <c r="T28" s="37"/>
+      <c r="U28" s="37"/>
     </row>
     <row r="29" spans="1:21">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
-      <c r="O29" s="2"/>
-      <c r="P29" s="2"/>
-      <c r="Q29" s="2"/>
-      <c r="R29" s="2"/>
-      <c r="S29" s="2"/>
-      <c r="T29" s="2"/>
-      <c r="U29" s="2"/>
+      <c r="A29" s="37"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="37"/>
+      <c r="K29" s="37"/>
+      <c r="L29" s="37"/>
+      <c r="M29" s="37"/>
+      <c r="N29" s="37"/>
+      <c r="O29" s="37"/>
+      <c r="P29" s="37"/>
+      <c r="Q29" s="37"/>
+      <c r="R29" s="37"/>
+      <c r="S29" s="37"/>
+      <c r="T29" s="37"/>
+      <c r="U29" s="37"/>
     </row>
     <row r="30" spans="1:21">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
-      <c r="O30" s="2"/>
-      <c r="P30" s="2"/>
-      <c r="Q30" s="2"/>
-      <c r="R30" s="2"/>
-      <c r="S30" s="2"/>
-      <c r="T30" s="2"/>
-      <c r="U30" s="2"/>
+      <c r="A30" s="37"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="37"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="37"/>
+      <c r="I30" s="37"/>
+      <c r="J30" s="37"/>
+      <c r="K30" s="37"/>
+      <c r="L30" s="37"/>
+      <c r="M30" s="37"/>
+      <c r="N30" s="37"/>
+      <c r="O30" s="37"/>
+      <c r="P30" s="37"/>
+      <c r="Q30" s="37"/>
+      <c r="R30" s="37"/>
+      <c r="S30" s="37"/>
+      <c r="T30" s="37"/>
+      <c r="U30" s="37"/>
     </row>
     <row r="31" spans="1:21">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
-      <c r="O31" s="2"/>
-      <c r="P31" s="2"/>
-      <c r="Q31" s="2"/>
-      <c r="R31" s="2"/>
-      <c r="S31" s="2"/>
-      <c r="T31" s="2"/>
-      <c r="U31" s="2"/>
+      <c r="A31" s="37"/>
+      <c r="B31" s="37"/>
+      <c r="C31" s="37"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="37"/>
+      <c r="G31" s="37"/>
+      <c r="H31" s="37"/>
+      <c r="I31" s="37"/>
+      <c r="J31" s="37"/>
+      <c r="K31" s="37"/>
+      <c r="L31" s="37"/>
+      <c r="M31" s="37"/>
+      <c r="N31" s="37"/>
+      <c r="O31" s="37"/>
+      <c r="P31" s="37"/>
+      <c r="Q31" s="37"/>
+      <c r="R31" s="37"/>
+      <c r="S31" s="37"/>
+      <c r="T31" s="37"/>
+      <c r="U31" s="37"/>
     </row>
     <row r="32" spans="1:21">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
-      <c r="O32" s="2"/>
-      <c r="P32" s="2"/>
-      <c r="Q32" s="2"/>
-      <c r="R32" s="2"/>
-      <c r="S32" s="2"/>
-      <c r="T32" s="2"/>
-      <c r="U32" s="2"/>
+      <c r="A32" s="37"/>
+      <c r="B32" s="37"/>
+      <c r="C32" s="37"/>
+      <c r="D32" s="37"/>
+      <c r="E32" s="37"/>
+      <c r="F32" s="37"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="37"/>
+      <c r="I32" s="37"/>
+      <c r="J32" s="37"/>
+      <c r="K32" s="37"/>
+      <c r="L32" s="37"/>
+      <c r="M32" s="37"/>
+      <c r="N32" s="37"/>
+      <c r="O32" s="37"/>
+      <c r="P32" s="37"/>
+      <c r="Q32" s="37"/>
+      <c r="R32" s="37"/>
+      <c r="S32" s="37"/>
+      <c r="T32" s="37"/>
+      <c r="U32" s="37"/>
     </row>
     <row r="33" spans="1:21">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
-      <c r="O33" s="2"/>
-      <c r="P33" s="2"/>
-      <c r="Q33" s="2"/>
-      <c r="R33" s="2"/>
-      <c r="S33" s="2"/>
-      <c r="T33" s="2"/>
-      <c r="U33" s="2"/>
+      <c r="A33" s="37"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="37"/>
+      <c r="D33" s="37"/>
+      <c r="E33" s="37"/>
+      <c r="F33" s="37"/>
+      <c r="G33" s="37"/>
+      <c r="H33" s="37"/>
+      <c r="I33" s="37"/>
+      <c r="J33" s="37"/>
+      <c r="K33" s="37"/>
+      <c r="L33" s="37"/>
+      <c r="M33" s="37"/>
+      <c r="N33" s="37"/>
+      <c r="O33" s="37"/>
+      <c r="P33" s="37"/>
+      <c r="Q33" s="37"/>
+      <c r="R33" s="37"/>
+      <c r="S33" s="37"/>
+      <c r="T33" s="37"/>
+      <c r="U33" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="H1:N1"/>
+    <mergeCell ref="O1:U1"/>
+    <mergeCell ref="A2:G11"/>
+    <mergeCell ref="H2:N11"/>
+    <mergeCell ref="O2:U11"/>
+    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="H12:N12"/>
+    <mergeCell ref="O12:U12"/>
+    <mergeCell ref="A13:G22"/>
+    <mergeCell ref="H13:N22"/>
+    <mergeCell ref="O13:U22"/>
     <mergeCell ref="A23:G23"/>
     <mergeCell ref="H23:N23"/>
     <mergeCell ref="O23:U23"/>
     <mergeCell ref="A24:G33"/>
     <mergeCell ref="H24:N33"/>
     <mergeCell ref="O24:U33"/>
-    <mergeCell ref="A12:G12"/>
-    <mergeCell ref="H12:N12"/>
-    <mergeCell ref="O12:U12"/>
-    <mergeCell ref="A13:G22"/>
-    <mergeCell ref="H13:N22"/>
-    <mergeCell ref="O13:U22"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="H1:N1"/>
-    <mergeCell ref="O1:U1"/>
-    <mergeCell ref="A2:G11"/>
-    <mergeCell ref="H2:N11"/>
-    <mergeCell ref="O2:U11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2728,34 +2919,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="19">
+      <c r="B1" s="13">
         <v>0.1</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="21">
+      <c r="D1" s="15">
         <f>B1*10^3</f>
         <v>100</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="22">
+      <c r="F1" s="16">
         <f>D1*10^3</f>
         <v>100000</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="23">
+      <c r="H1" s="17">
         <f>D1*10^6</f>
         <v>100000000</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="17" t="s">
         <v>80</v>
       </c>
       <c r="S1" t="s">
@@ -2763,126 +2954,126 @@
       </c>
     </row>
     <row r="2" spans="1:19">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="20">
+      <c r="B2" s="14">
         <f>1/B1</f>
         <v>10</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="D2" s="21">
+      <c r="D2" s="15">
         <f>B2/10^3</f>
         <v>0.01</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="F2" s="22">
+      <c r="F2" s="16">
         <f>B2/10^6</f>
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="H2" s="23">
+      <c r="H2" s="17">
         <f>F2/10^3</f>
         <v>1E-8</v>
       </c>
-      <c r="I2" s="23" t="s">
+      <c r="I2" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="L2" s="24" t="s">
+      <c r="L2" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="M2" s="24" t="s">
+      <c r="M2" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
     </row>
     <row r="3" spans="1:19">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="B3" s="25">
+      <c r="B3" s="19">
         <f>(F3*10^6)</f>
         <v>80000000</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="D3" s="26">
+      <c r="D3" s="20">
         <f>B3/10^3</f>
         <v>80000</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="13">
         <v>80</v>
       </c>
-      <c r="G3" s="27" t="s">
+      <c r="G3" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="H3" s="28">
+      <c r="H3" s="22">
         <f>F3/10^3</f>
         <v>0.08</v>
       </c>
-      <c r="I3" s="28" t="s">
+      <c r="I3" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="L3" s="24" t="s">
+      <c r="L3" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="M3" s="24" t="s">
+      <c r="M3" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
     </row>
     <row r="4" spans="1:19">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="B4" s="29">
+      <c r="B4" s="23">
         <f>1/B3</f>
         <v>1.2499999999999999E-8</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="30">
+      <c r="D4" s="24">
         <f>B4*10^3</f>
         <v>1.2499999999999999E-5</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="F4" s="31">
+      <c r="F4" s="25">
         <f>D4*10^3</f>
         <v>1.2499999999999999E-2</v>
       </c>
-      <c r="G4" s="31" t="s">
+      <c r="G4" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="H4" s="32">
+      <c r="H4" s="26">
         <f>B4*10^9</f>
         <v>12.5</v>
       </c>
-      <c r="I4" s="32" t="s">
+      <c r="I4" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="L4" s="24" t="s">
+      <c r="L4" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="M4" s="24" t="s">
+      <c r="M4" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="N4" s="24"/>
-      <c r="O4" s="24"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
     </row>
     <row r="5" spans="1:19">
       <c r="H5">
@@ -2891,15 +3082,15 @@
       </c>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="B6" s="34">
+      <c r="B6" s="28">
         <f>(H1/H4)-1</f>
         <v>7999999</v>
       </c>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
       <c r="E6" t="s">
         <v>96</v>
       </c>
@@ -2909,10 +3100,10 @@
       </c>
     </row>
     <row r="7" spans="1:19">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="B7" s="34" t="str">
+      <c r="B7" s="28" t="str">
         <f>DEC2HEX(B6)</f>
         <v>7A11FF</v>
       </c>
@@ -2922,7 +3113,7 @@
       <c r="F7">
         <v>5000</v>
       </c>
-      <c r="H7" s="36"/>
+      <c r="H7" s="30"/>
     </row>
     <row r="8" spans="1:19">
       <c r="E8" t="s">
@@ -2933,7 +3124,7 @@
       </c>
     </row>
     <row r="9" spans="1:19">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="31" t="s">
         <v>100</v>
       </c>
       <c r="B9">
@@ -2941,12 +3132,12 @@
       </c>
     </row>
     <row r="12" spans="1:19" ht="15.75">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="32" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="15.75">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="32" t="s">
         <v>102</v>
       </c>
     </row>
@@ -2958,16 +3149,332 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="40" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" s="40" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="E2" s="39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="E3" s="39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" s="39" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="D4" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="E4" s="39">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>115</v>
+      </c>
+      <c r="D5" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="E5" s="39">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="39" t="s">
+        <v>132</v>
+      </c>
+      <c r="B6" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="D6" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="E6" s="39">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="39" t="s">
+        <v>133</v>
+      </c>
+      <c r="B7" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>124</v>
+      </c>
+      <c r="D7" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="E7" s="39">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="39" t="s">
+        <v>134</v>
+      </c>
+      <c r="B8" s="39" t="s">
+        <v>126</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>125</v>
+      </c>
+      <c r="D8" s="39" t="s">
+        <v>127</v>
+      </c>
+      <c r="E8" s="39">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="39" t="s">
+        <v>135</v>
+      </c>
+      <c r="B9" s="39" t="s">
+        <v>150</v>
+      </c>
+      <c r="C9" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="B10" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="C10" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="39" t="s">
+        <v>137</v>
+      </c>
+      <c r="B11" s="39" t="s">
+        <v>155</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="39" t="s">
+        <v>138</v>
+      </c>
+      <c r="B12" s="39" t="s">
+        <v>156</v>
+      </c>
+      <c r="C12" s="39" t="s">
+        <v>158</v>
+      </c>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="B13" s="39"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="39" t="s">
+        <v>140</v>
+      </c>
+      <c r="B14" s="39"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="B15" s="39"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="39" t="s">
+        <v>142</v>
+      </c>
+      <c r="B16" s="39"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="39" t="s">
+        <v>143</v>
+      </c>
+      <c r="B17" s="39"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="39" t="s">
+        <v>144</v>
+      </c>
+      <c r="B18" s="39"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="39" t="s">
+        <v>145</v>
+      </c>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="39" t="s">
+        <v>146</v>
+      </c>
+      <c r="B20" s="39"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="39"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="39" t="s">
+        <v>147</v>
+      </c>
+      <c r="B21" s="39"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="39"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="39" t="s">
+        <v>148</v>
+      </c>
+      <c r="B22" s="39"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="39"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="39" t="s">
+        <v>149</v>
+      </c>
+      <c r="B23" s="39"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="41" t="s">
+        <v>153</v>
+      </c>
+      <c r="B24" s="41" t="s">
+        <v>154</v>
+      </c>
+      <c r="C24" s="41"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="41">
+        <v>254</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:E24"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
integrating SMS receive functionality
for some unknown reason the data on UART from GSM module is sporadic
investigate if its a RTOS issue
</commit_message>
<xml_diff>
--- a/SecSys_TM4C/SecSys.xlsx
+++ b/SecSys_TM4C/SecSys.xlsx
@@ -4,16 +4,17 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Pin Map" sheetId="1" r:id="rId1"/>
     <sheet name="TODO" sheetId="2" r:id="rId2"/>
     <sheet name="Timer Reload Value" sheetId="3" r:id="rId3"/>
     <sheet name="OS Tasks" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'OS Tasks'!$A$1:$E$24</definedName>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="161">
   <si>
     <t>Port / Pin</t>
   </si>
@@ -669,6 +670,12 @@
   </si>
   <si>
     <t>SemPortF.pin4</t>
+  </si>
+  <si>
+    <t>SW2 = PF0</t>
+  </si>
+  <si>
+    <t>SW1 = PF4</t>
   </si>
 </sst>
 </file>
@@ -1023,13 +1030,16 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1041,9 +1051,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -1120,6 +1127,56 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>62802</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>83737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>471016</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>31402</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1025" name="Picture 1" descr="http://energia.nu/wordpress/wp-content/uploads/2014/01/LaunchPads-LM4F-TM4C-%E2%80%94-Pins-Maps-11-32.jpeg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email"/>
+        <a:srcRect l="4273" t="14465" r="4228" b="10402"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="62802" y="83737"/>
+          <a:ext cx="12549972" cy="5599863"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1446,8 +1503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1492,7 +1549,7 @@
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="37" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1515,7 +1572,7 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="34"/>
+      <c r="A4" s="37"/>
       <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
@@ -1536,7 +1593,7 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="34"/>
+      <c r="A5" s="37"/>
       <c r="B5" s="4" t="s">
         <v>15</v>
       </c>
@@ -1547,7 +1604,7 @@
       <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="34"/>
+      <c r="A6" s="37"/>
       <c r="B6" s="4" t="s">
         <v>16</v>
       </c>
@@ -1558,7 +1615,7 @@
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="34"/>
+      <c r="A7" s="37"/>
       <c r="B7" s="4" t="s">
         <v>17</v>
       </c>
@@ -1569,7 +1626,7 @@
       <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="34"/>
+      <c r="A8" s="37"/>
       <c r="B8" s="4" t="s">
         <v>18</v>
       </c>
@@ -1580,7 +1637,7 @@
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="34"/>
+      <c r="A9" s="37"/>
       <c r="B9" s="4" t="s">
         <v>19</v>
       </c>
@@ -1591,7 +1648,7 @@
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="34"/>
+      <c r="A10" s="37"/>
       <c r="B10" s="4" t="s">
         <v>20</v>
       </c>
@@ -1611,7 +1668,7 @@
       <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="37" t="s">
         <v>21</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -1624,7 +1681,7 @@
       <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="34"/>
+      <c r="A13" s="37"/>
       <c r="B13" s="4" t="s">
         <v>23</v>
       </c>
@@ -1635,7 +1692,7 @@
       <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="34"/>
+      <c r="A14" s="37"/>
       <c r="B14" s="4" t="s">
         <v>24</v>
       </c>
@@ -1646,7 +1703,7 @@
       <c r="G14" s="4"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="34"/>
+      <c r="A15" s="37"/>
       <c r="B15" s="4" t="s">
         <v>25</v>
       </c>
@@ -1657,7 +1714,7 @@
       <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="34"/>
+      <c r="A16" s="37"/>
       <c r="B16" s="4" t="s">
         <v>26</v>
       </c>
@@ -1668,7 +1725,7 @@
       <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="34"/>
+      <c r="A17" s="37"/>
       <c r="B17" s="4" t="s">
         <v>27</v>
       </c>
@@ -1679,7 +1736,7 @@
       <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="34"/>
+      <c r="A18" s="37"/>
       <c r="B18" s="4" t="s">
         <v>28</v>
       </c>
@@ -1699,47 +1756,47 @@
       <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="34" t="s">
+      <c r="A20" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="35"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="36"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="34"/>
-      <c r="B21" s="35"/>
-      <c r="C21" s="35"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="35"/>
+      <c r="A21" s="37"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="34"/>
-      <c r="B22" s="35"/>
-      <c r="C22" s="35"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="35"/>
+      <c r="A22" s="37"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="34"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="35"/>
+      <c r="A23" s="37"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="34"/>
+      <c r="A24" s="37"/>
       <c r="B24" s="8" t="s">
         <v>31</v>
       </c>
@@ -1750,7 +1807,7 @@
       <c r="G24" s="8"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="34"/>
+      <c r="A25" s="37"/>
       <c r="B25" s="8" t="s">
         <v>32</v>
       </c>
@@ -1761,7 +1818,7 @@
       <c r="G25" s="8"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="34"/>
+      <c r="A26" s="37"/>
       <c r="B26" s="8" t="s">
         <v>33</v>
       </c>
@@ -1782,7 +1839,7 @@
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="34"/>
+      <c r="A27" s="37"/>
       <c r="B27" s="8" t="s">
         <v>39</v>
       </c>
@@ -1812,7 +1869,7 @@
       <c r="G28" s="3"/>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="34" t="s">
+      <c r="A29" s="37" t="s">
         <v>41</v>
       </c>
       <c r="B29" s="5" t="s">
@@ -1825,7 +1882,7 @@
       <c r="G29" s="5"/>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="34"/>
+      <c r="A30" s="37"/>
       <c r="B30" s="5" t="s">
         <v>43</v>
       </c>
@@ -1836,7 +1893,7 @@
       <c r="G30" s="5"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="34"/>
+      <c r="A31" s="37"/>
       <c r="B31" s="5" t="s">
         <v>44</v>
       </c>
@@ -1847,7 +1904,7 @@
       <c r="G31" s="5"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="34"/>
+      <c r="A32" s="37"/>
       <c r="B32" s="5" t="s">
         <v>45</v>
       </c>
@@ -1858,7 +1915,7 @@
       <c r="G32" s="5"/>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="34"/>
+      <c r="A33" s="37"/>
       <c r="B33" s="9" t="s">
         <v>46</v>
       </c>
@@ -1879,7 +1936,7 @@
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="34"/>
+      <c r="A34" s="37"/>
       <c r="B34" s="4" t="s">
         <v>49</v>
       </c>
@@ -1909,7 +1966,7 @@
       <c r="G35" s="3"/>
     </row>
     <row r="36" spans="1:7" ht="15" customHeight="1">
-      <c r="A36" s="33" t="s">
+      <c r="A36" s="38" t="s">
         <v>51</v>
       </c>
       <c r="B36" s="9" t="s">
@@ -1922,7 +1979,7 @@
       <c r="G36" s="4"/>
     </row>
     <row r="37" spans="1:7" ht="15" customHeight="1">
-      <c r="A37" s="33"/>
+      <c r="A37" s="38"/>
       <c r="B37" s="4" t="s">
         <v>53</v>
       </c>
@@ -1937,7 +1994,7 @@
       <c r="G37" s="4"/>
     </row>
     <row r="38" spans="1:7" ht="15" customHeight="1">
-      <c r="A38" s="33"/>
+      <c r="A38" s="38"/>
       <c r="B38" s="4" t="s">
         <v>55</v>
       </c>
@@ -1952,7 +2009,7 @@
       <c r="G38" s="4"/>
     </row>
     <row r="39" spans="1:7" ht="15" customHeight="1">
-      <c r="A39" s="33"/>
+      <c r="A39" s="38"/>
       <c r="B39" s="4" t="s">
         <v>57</v>
       </c>
@@ -1967,7 +2024,7 @@
       <c r="G39" s="4"/>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="33"/>
+      <c r="A40" s="38"/>
       <c r="B40" s="4" t="s">
         <v>59</v>
       </c>
@@ -1978,7 +2035,7 @@
       <c r="G40" s="4"/>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="33"/>
+      <c r="A41" s="38"/>
       <c r="B41" s="4" t="s">
         <v>60</v>
       </c>
@@ -1998,7 +2055,7 @@
       <c r="G42" s="3"/>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="34" t="s">
+      <c r="A43" s="37" t="s">
         <v>61</v>
       </c>
       <c r="B43" s="4" t="s">
@@ -2011,7 +2068,7 @@
       <c r="G43" s="4"/>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="34"/>
+      <c r="A44" s="37"/>
       <c r="B44" s="6" t="s">
         <v>63</v>
       </c>
@@ -2022,7 +2079,7 @@
       <c r="G44" s="4"/>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="34"/>
+      <c r="A45" s="37"/>
       <c r="B45" s="10" t="s">
         <v>64</v>
       </c>
@@ -2033,7 +2090,7 @@
       <c r="G45" s="4"/>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="34"/>
+      <c r="A46" s="37"/>
       <c r="B46" s="11" t="s">
         <v>65</v>
       </c>
@@ -2044,7 +2101,7 @@
       <c r="G46" s="4"/>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="34"/>
+      <c r="A47" s="37"/>
       <c r="B47" s="4" t="s">
         <v>66</v>
       </c>
@@ -2082,8 +2139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U33"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23:U23"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="X17" sqref="X17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2092,802 +2149,802 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36" t="s">
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36" t="s">
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
-      <c r="S1" s="36"/>
-      <c r="T1" s="36"/>
-      <c r="U1" s="36"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="39"/>
+      <c r="R1" s="39"/>
+      <c r="S1" s="39"/>
+      <c r="T1" s="39"/>
+      <c r="U1" s="39"/>
     </row>
     <row r="2" spans="1:21" ht="15" customHeight="1">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="38" t="s">
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="37"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="37"/>
-      <c r="U2" s="37"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="40"/>
+      <c r="S2" s="40"/>
+      <c r="T2" s="40"/>
+      <c r="U2" s="40"/>
     </row>
     <row r="3" spans="1:21">
-      <c r="A3" s="37"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
-      <c r="N3" s="38"/>
-      <c r="O3" s="37"/>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="37"/>
-      <c r="R3" s="37"/>
-      <c r="S3" s="37"/>
-      <c r="T3" s="37"/>
-      <c r="U3" s="37"/>
+      <c r="A3" s="40"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="41"/>
+      <c r="O3" s="40"/>
+      <c r="P3" s="40"/>
+      <c r="Q3" s="40"/>
+      <c r="R3" s="40"/>
+      <c r="S3" s="40"/>
+      <c r="T3" s="40"/>
+      <c r="U3" s="40"/>
     </row>
     <row r="4" spans="1:21">
-      <c r="A4" s="37"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
-      <c r="K4" s="38"/>
-      <c r="L4" s="38"/>
-      <c r="M4" s="38"/>
-      <c r="N4" s="38"/>
-      <c r="O4" s="37"/>
-      <c r="P4" s="37"/>
-      <c r="Q4" s="37"/>
-      <c r="R4" s="37"/>
-      <c r="S4" s="37"/>
-      <c r="T4" s="37"/>
-      <c r="U4" s="37"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="41"/>
+      <c r="L4" s="41"/>
+      <c r="M4" s="41"/>
+      <c r="N4" s="41"/>
+      <c r="O4" s="40"/>
+      <c r="P4" s="40"/>
+      <c r="Q4" s="40"/>
+      <c r="R4" s="40"/>
+      <c r="S4" s="40"/>
+      <c r="T4" s="40"/>
+      <c r="U4" s="40"/>
     </row>
     <row r="5" spans="1:21">
-      <c r="A5" s="37"/>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="38"/>
-      <c r="M5" s="38"/>
-      <c r="N5" s="38"/>
-      <c r="O5" s="37"/>
-      <c r="P5" s="37"/>
-      <c r="Q5" s="37"/>
-      <c r="R5" s="37"/>
-      <c r="S5" s="37"/>
-      <c r="T5" s="37"/>
-      <c r="U5" s="37"/>
+      <c r="A5" s="40"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="41"/>
+      <c r="N5" s="41"/>
+      <c r="O5" s="40"/>
+      <c r="P5" s="40"/>
+      <c r="Q5" s="40"/>
+      <c r="R5" s="40"/>
+      <c r="S5" s="40"/>
+      <c r="T5" s="40"/>
+      <c r="U5" s="40"/>
     </row>
     <row r="6" spans="1:21">
-      <c r="A6" s="37"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
-      <c r="K6" s="38"/>
-      <c r="L6" s="38"/>
-      <c r="M6" s="38"/>
-      <c r="N6" s="38"/>
-      <c r="O6" s="37"/>
-      <c r="P6" s="37"/>
-      <c r="Q6" s="37"/>
-      <c r="R6" s="37"/>
-      <c r="S6" s="37"/>
-      <c r="T6" s="37"/>
-      <c r="U6" s="37"/>
+      <c r="A6" s="40"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="41"/>
+      <c r="N6" s="41"/>
+      <c r="O6" s="40"/>
+      <c r="P6" s="40"/>
+      <c r="Q6" s="40"/>
+      <c r="R6" s="40"/>
+      <c r="S6" s="40"/>
+      <c r="T6" s="40"/>
+      <c r="U6" s="40"/>
     </row>
     <row r="7" spans="1:21">
-      <c r="A7" s="37"/>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="38"/>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38"/>
-      <c r="M7" s="38"/>
-      <c r="N7" s="38"/>
-      <c r="O7" s="37"/>
-      <c r="P7" s="37"/>
-      <c r="Q7" s="37"/>
-      <c r="R7" s="37"/>
-      <c r="S7" s="37"/>
-      <c r="T7" s="37"/>
-      <c r="U7" s="37"/>
+      <c r="A7" s="40"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="41"/>
+      <c r="M7" s="41"/>
+      <c r="N7" s="41"/>
+      <c r="O7" s="40"/>
+      <c r="P7" s="40"/>
+      <c r="Q7" s="40"/>
+      <c r="R7" s="40"/>
+      <c r="S7" s="40"/>
+      <c r="T7" s="40"/>
+      <c r="U7" s="40"/>
     </row>
     <row r="8" spans="1:21">
-      <c r="A8" s="37"/>
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
-      <c r="J8" s="38"/>
-      <c r="K8" s="38"/>
-      <c r="L8" s="38"/>
-      <c r="M8" s="38"/>
-      <c r="N8" s="38"/>
-      <c r="O8" s="37"/>
-      <c r="P8" s="37"/>
-      <c r="Q8" s="37"/>
-      <c r="R8" s="37"/>
-      <c r="S8" s="37"/>
-      <c r="T8" s="37"/>
-      <c r="U8" s="37"/>
+      <c r="A8" s="40"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="41"/>
+      <c r="M8" s="41"/>
+      <c r="N8" s="41"/>
+      <c r="O8" s="40"/>
+      <c r="P8" s="40"/>
+      <c r="Q8" s="40"/>
+      <c r="R8" s="40"/>
+      <c r="S8" s="40"/>
+      <c r="T8" s="40"/>
+      <c r="U8" s="40"/>
     </row>
     <row r="9" spans="1:21">
-      <c r="A9" s="37"/>
-      <c r="B9" s="37"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="38"/>
-      <c r="K9" s="38"/>
-      <c r="L9" s="38"/>
-      <c r="M9" s="38"/>
-      <c r="N9" s="38"/>
-      <c r="O9" s="37"/>
-      <c r="P9" s="37"/>
-      <c r="Q9" s="37"/>
-      <c r="R9" s="37"/>
-      <c r="S9" s="37"/>
-      <c r="T9" s="37"/>
-      <c r="U9" s="37"/>
+      <c r="A9" s="40"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="41"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="41"/>
+      <c r="M9" s="41"/>
+      <c r="N9" s="41"/>
+      <c r="O9" s="40"/>
+      <c r="P9" s="40"/>
+      <c r="Q9" s="40"/>
+      <c r="R9" s="40"/>
+      <c r="S9" s="40"/>
+      <c r="T9" s="40"/>
+      <c r="U9" s="40"/>
     </row>
     <row r="10" spans="1:21">
-      <c r="A10" s="37"/>
-      <c r="B10" s="37"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="38"/>
-      <c r="M10" s="38"/>
-      <c r="N10" s="38"/>
-      <c r="O10" s="37"/>
-      <c r="P10" s="37"/>
-      <c r="Q10" s="37"/>
-      <c r="R10" s="37"/>
-      <c r="S10" s="37"/>
-      <c r="T10" s="37"/>
-      <c r="U10" s="37"/>
+      <c r="A10" s="40"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="41"/>
+      <c r="M10" s="41"/>
+      <c r="N10" s="41"/>
+      <c r="O10" s="40"/>
+      <c r="P10" s="40"/>
+      <c r="Q10" s="40"/>
+      <c r="R10" s="40"/>
+      <c r="S10" s="40"/>
+      <c r="T10" s="40"/>
+      <c r="U10" s="40"/>
     </row>
     <row r="11" spans="1:21">
-      <c r="A11" s="37"/>
-      <c r="B11" s="37"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="38"/>
-      <c r="L11" s="38"/>
-      <c r="M11" s="38"/>
-      <c r="N11" s="38"/>
-      <c r="O11" s="37"/>
-      <c r="P11" s="37"/>
-      <c r="Q11" s="37"/>
-      <c r="R11" s="37"/>
-      <c r="S11" s="37"/>
-      <c r="T11" s="37"/>
-      <c r="U11" s="37"/>
+      <c r="A11" s="40"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="41"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="41"/>
+      <c r="M11" s="41"/>
+      <c r="N11" s="41"/>
+      <c r="O11" s="40"/>
+      <c r="P11" s="40"/>
+      <c r="Q11" s="40"/>
+      <c r="R11" s="40"/>
+      <c r="S11" s="40"/>
+      <c r="T11" s="40"/>
+      <c r="U11" s="40"/>
     </row>
     <row r="12" spans="1:21">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36" t="s">
+      <c r="B12" s="39"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="I12" s="36"/>
-      <c r="J12" s="36"/>
-      <c r="K12" s="36"/>
-      <c r="L12" s="36"/>
-      <c r="M12" s="36"/>
-      <c r="N12" s="36"/>
-      <c r="O12" s="36"/>
-      <c r="P12" s="36"/>
-      <c r="Q12" s="36"/>
-      <c r="R12" s="36"/>
-      <c r="S12" s="36"/>
-      <c r="T12" s="36"/>
-      <c r="U12" s="36"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="39"/>
+      <c r="L12" s="39"/>
+      <c r="M12" s="39"/>
+      <c r="N12" s="39"/>
+      <c r="O12" s="39"/>
+      <c r="P12" s="39"/>
+      <c r="Q12" s="39"/>
+      <c r="R12" s="39"/>
+      <c r="S12" s="39"/>
+      <c r="T12" s="39"/>
+      <c r="U12" s="39"/>
     </row>
     <row r="13" spans="1:21" ht="15" customHeight="1">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37" t="s">
+      <c r="B13" s="40"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="I13" s="37"/>
-      <c r="J13" s="37"/>
-      <c r="K13" s="37"/>
-      <c r="L13" s="37"/>
-      <c r="M13" s="37"/>
-      <c r="N13" s="37"/>
-      <c r="O13" s="37"/>
-      <c r="P13" s="37"/>
-      <c r="Q13" s="37"/>
-      <c r="R13" s="37"/>
-      <c r="S13" s="37"/>
-      <c r="T13" s="37"/>
-      <c r="U13" s="37"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="40"/>
+      <c r="L13" s="40"/>
+      <c r="M13" s="40"/>
+      <c r="N13" s="40"/>
+      <c r="O13" s="40"/>
+      <c r="P13" s="40"/>
+      <c r="Q13" s="40"/>
+      <c r="R13" s="40"/>
+      <c r="S13" s="40"/>
+      <c r="T13" s="40"/>
+      <c r="U13" s="40"/>
     </row>
     <row r="14" spans="1:21">
-      <c r="A14" s="37"/>
-      <c r="B14" s="37"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="37"/>
-      <c r="K14" s="37"/>
-      <c r="L14" s="37"/>
-      <c r="M14" s="37"/>
-      <c r="N14" s="37"/>
-      <c r="O14" s="37"/>
-      <c r="P14" s="37"/>
-      <c r="Q14" s="37"/>
-      <c r="R14" s="37"/>
-      <c r="S14" s="37"/>
-      <c r="T14" s="37"/>
-      <c r="U14" s="37"/>
+      <c r="A14" s="40"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="40"/>
+      <c r="L14" s="40"/>
+      <c r="M14" s="40"/>
+      <c r="N14" s="40"/>
+      <c r="O14" s="40"/>
+      <c r="P14" s="40"/>
+      <c r="Q14" s="40"/>
+      <c r="R14" s="40"/>
+      <c r="S14" s="40"/>
+      <c r="T14" s="40"/>
+      <c r="U14" s="40"/>
     </row>
     <row r="15" spans="1:21">
-      <c r="A15" s="37"/>
-      <c r="B15" s="37"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="37"/>
-      <c r="K15" s="37"/>
-      <c r="L15" s="37"/>
-      <c r="M15" s="37"/>
-      <c r="N15" s="37"/>
-      <c r="O15" s="37"/>
-      <c r="P15" s="37"/>
-      <c r="Q15" s="37"/>
-      <c r="R15" s="37"/>
-      <c r="S15" s="37"/>
-      <c r="T15" s="37"/>
-      <c r="U15" s="37"/>
+      <c r="A15" s="40"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="40"/>
+      <c r="K15" s="40"/>
+      <c r="L15" s="40"/>
+      <c r="M15" s="40"/>
+      <c r="N15" s="40"/>
+      <c r="O15" s="40"/>
+      <c r="P15" s="40"/>
+      <c r="Q15" s="40"/>
+      <c r="R15" s="40"/>
+      <c r="S15" s="40"/>
+      <c r="T15" s="40"/>
+      <c r="U15" s="40"/>
     </row>
     <row r="16" spans="1:21">
-      <c r="A16" s="37"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="37"/>
-      <c r="K16" s="37"/>
-      <c r="L16" s="37"/>
-      <c r="M16" s="37"/>
-      <c r="N16" s="37"/>
-      <c r="O16" s="37"/>
-      <c r="P16" s="37"/>
-      <c r="Q16" s="37"/>
-      <c r="R16" s="37"/>
-      <c r="S16" s="37"/>
-      <c r="T16" s="37"/>
-      <c r="U16" s="37"/>
+      <c r="A16" s="40"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
+      <c r="K16" s="40"/>
+      <c r="L16" s="40"/>
+      <c r="M16" s="40"/>
+      <c r="N16" s="40"/>
+      <c r="O16" s="40"/>
+      <c r="P16" s="40"/>
+      <c r="Q16" s="40"/>
+      <c r="R16" s="40"/>
+      <c r="S16" s="40"/>
+      <c r="T16" s="40"/>
+      <c r="U16" s="40"/>
     </row>
     <row r="17" spans="1:21">
-      <c r="A17" s="37"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="37"/>
-      <c r="J17" s="37"/>
-      <c r="K17" s="37"/>
-      <c r="L17" s="37"/>
-      <c r="M17" s="37"/>
-      <c r="N17" s="37"/>
-      <c r="O17" s="37"/>
-      <c r="P17" s="37"/>
-      <c r="Q17" s="37"/>
-      <c r="R17" s="37"/>
-      <c r="S17" s="37"/>
-      <c r="T17" s="37"/>
-      <c r="U17" s="37"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="40"/>
+      <c r="L17" s="40"/>
+      <c r="M17" s="40"/>
+      <c r="N17" s="40"/>
+      <c r="O17" s="40"/>
+      <c r="P17" s="40"/>
+      <c r="Q17" s="40"/>
+      <c r="R17" s="40"/>
+      <c r="S17" s="40"/>
+      <c r="T17" s="40"/>
+      <c r="U17" s="40"/>
     </row>
     <row r="18" spans="1:21">
-      <c r="A18" s="37"/>
-      <c r="B18" s="37"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="37"/>
-      <c r="K18" s="37"/>
-      <c r="L18" s="37"/>
-      <c r="M18" s="37"/>
-      <c r="N18" s="37"/>
-      <c r="O18" s="37"/>
-      <c r="P18" s="37"/>
-      <c r="Q18" s="37"/>
-      <c r="R18" s="37"/>
-      <c r="S18" s="37"/>
-      <c r="T18" s="37"/>
-      <c r="U18" s="37"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
+      <c r="K18" s="40"/>
+      <c r="L18" s="40"/>
+      <c r="M18" s="40"/>
+      <c r="N18" s="40"/>
+      <c r="O18" s="40"/>
+      <c r="P18" s="40"/>
+      <c r="Q18" s="40"/>
+      <c r="R18" s="40"/>
+      <c r="S18" s="40"/>
+      <c r="T18" s="40"/>
+      <c r="U18" s="40"/>
     </row>
     <row r="19" spans="1:21">
-      <c r="A19" s="37"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
-      <c r="K19" s="37"/>
-      <c r="L19" s="37"/>
-      <c r="M19" s="37"/>
-      <c r="N19" s="37"/>
-      <c r="O19" s="37"/>
-      <c r="P19" s="37"/>
-      <c r="Q19" s="37"/>
-      <c r="R19" s="37"/>
-      <c r="S19" s="37"/>
-      <c r="T19" s="37"/>
-      <c r="U19" s="37"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="40"/>
+      <c r="L19" s="40"/>
+      <c r="M19" s="40"/>
+      <c r="N19" s="40"/>
+      <c r="O19" s="40"/>
+      <c r="P19" s="40"/>
+      <c r="Q19" s="40"/>
+      <c r="R19" s="40"/>
+      <c r="S19" s="40"/>
+      <c r="T19" s="40"/>
+      <c r="U19" s="40"/>
     </row>
     <row r="20" spans="1:21">
-      <c r="A20" s="37"/>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="37"/>
-      <c r="J20" s="37"/>
-      <c r="K20" s="37"/>
-      <c r="L20" s="37"/>
-      <c r="M20" s="37"/>
-      <c r="N20" s="37"/>
-      <c r="O20" s="37"/>
-      <c r="P20" s="37"/>
-      <c r="Q20" s="37"/>
-      <c r="R20" s="37"/>
-      <c r="S20" s="37"/>
-      <c r="T20" s="37"/>
-      <c r="U20" s="37"/>
+      <c r="A20" s="40"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="40"/>
+      <c r="J20" s="40"/>
+      <c r="K20" s="40"/>
+      <c r="L20" s="40"/>
+      <c r="M20" s="40"/>
+      <c r="N20" s="40"/>
+      <c r="O20" s="40"/>
+      <c r="P20" s="40"/>
+      <c r="Q20" s="40"/>
+      <c r="R20" s="40"/>
+      <c r="S20" s="40"/>
+      <c r="T20" s="40"/>
+      <c r="U20" s="40"/>
     </row>
     <row r="21" spans="1:21">
-      <c r="A21" s="37"/>
-      <c r="B21" s="37"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="37"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="37"/>
-      <c r="I21" s="37"/>
-      <c r="J21" s="37"/>
-      <c r="K21" s="37"/>
-      <c r="L21" s="37"/>
-      <c r="M21" s="37"/>
-      <c r="N21" s="37"/>
-      <c r="O21" s="37"/>
-      <c r="P21" s="37"/>
-      <c r="Q21" s="37"/>
-      <c r="R21" s="37"/>
-      <c r="S21" s="37"/>
-      <c r="T21" s="37"/>
-      <c r="U21" s="37"/>
+      <c r="A21" s="40"/>
+      <c r="B21" s="40"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="40"/>
+      <c r="L21" s="40"/>
+      <c r="M21" s="40"/>
+      <c r="N21" s="40"/>
+      <c r="O21" s="40"/>
+      <c r="P21" s="40"/>
+      <c r="Q21" s="40"/>
+      <c r="R21" s="40"/>
+      <c r="S21" s="40"/>
+      <c r="T21" s="40"/>
+      <c r="U21" s="40"/>
     </row>
     <row r="22" spans="1:21">
-      <c r="A22" s="37"/>
-      <c r="B22" s="37"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="37"/>
-      <c r="H22" s="37"/>
-      <c r="I22" s="37"/>
-      <c r="J22" s="37"/>
-      <c r="K22" s="37"/>
-      <c r="L22" s="37"/>
-      <c r="M22" s="37"/>
-      <c r="N22" s="37"/>
-      <c r="O22" s="37"/>
-      <c r="P22" s="37"/>
-      <c r="Q22" s="37"/>
-      <c r="R22" s="37"/>
-      <c r="S22" s="37"/>
-      <c r="T22" s="37"/>
-      <c r="U22" s="37"/>
+      <c r="A22" s="40"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="40"/>
+      <c r="J22" s="40"/>
+      <c r="K22" s="40"/>
+      <c r="L22" s="40"/>
+      <c r="M22" s="40"/>
+      <c r="N22" s="40"/>
+      <c r="O22" s="40"/>
+      <c r="P22" s="40"/>
+      <c r="Q22" s="40"/>
+      <c r="R22" s="40"/>
+      <c r="S22" s="40"/>
+      <c r="T22" s="40"/>
+      <c r="U22" s="40"/>
     </row>
     <row r="23" spans="1:21">
-      <c r="A23" s="36"/>
-      <c r="B23" s="36"/>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="36"/>
-      <c r="J23" s="36"/>
-      <c r="K23" s="36"/>
-      <c r="L23" s="36"/>
-      <c r="M23" s="36"/>
-      <c r="N23" s="36"/>
-      <c r="O23" s="36"/>
-      <c r="P23" s="36"/>
-      <c r="Q23" s="36"/>
-      <c r="R23" s="36"/>
-      <c r="S23" s="36"/>
-      <c r="T23" s="36"/>
-      <c r="U23" s="36"/>
+      <c r="A23" s="39"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="39"/>
+      <c r="L23" s="39"/>
+      <c r="M23" s="39"/>
+      <c r="N23" s="39"/>
+      <c r="O23" s="39"/>
+      <c r="P23" s="39"/>
+      <c r="Q23" s="39"/>
+      <c r="R23" s="39"/>
+      <c r="S23" s="39"/>
+      <c r="T23" s="39"/>
+      <c r="U23" s="39"/>
     </row>
     <row r="24" spans="1:21">
-      <c r="A24" s="37"/>
-      <c r="B24" s="37"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="37"/>
-      <c r="H24" s="37"/>
-      <c r="I24" s="37"/>
-      <c r="J24" s="37"/>
-      <c r="K24" s="37"/>
-      <c r="L24" s="37"/>
-      <c r="M24" s="37"/>
-      <c r="N24" s="37"/>
-      <c r="O24" s="37"/>
-      <c r="P24" s="37"/>
-      <c r="Q24" s="37"/>
-      <c r="R24" s="37"/>
-      <c r="S24" s="37"/>
-      <c r="T24" s="37"/>
-      <c r="U24" s="37"/>
+      <c r="A24" s="40"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
+      <c r="K24" s="40"/>
+      <c r="L24" s="40"/>
+      <c r="M24" s="40"/>
+      <c r="N24" s="40"/>
+      <c r="O24" s="40"/>
+      <c r="P24" s="40"/>
+      <c r="Q24" s="40"/>
+      <c r="R24" s="40"/>
+      <c r="S24" s="40"/>
+      <c r="T24" s="40"/>
+      <c r="U24" s="40"/>
     </row>
     <row r="25" spans="1:21">
-      <c r="A25" s="37"/>
-      <c r="B25" s="37"/>
-      <c r="C25" s="37"/>
-      <c r="D25" s="37"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="37"/>
-      <c r="H25" s="37"/>
-      <c r="I25" s="37"/>
-      <c r="J25" s="37"/>
-      <c r="K25" s="37"/>
-      <c r="L25" s="37"/>
-      <c r="M25" s="37"/>
-      <c r="N25" s="37"/>
-      <c r="O25" s="37"/>
-      <c r="P25" s="37"/>
-      <c r="Q25" s="37"/>
-      <c r="R25" s="37"/>
-      <c r="S25" s="37"/>
-      <c r="T25" s="37"/>
-      <c r="U25" s="37"/>
+      <c r="A25" s="40"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="40"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="40"/>
+      <c r="L25" s="40"/>
+      <c r="M25" s="40"/>
+      <c r="N25" s="40"/>
+      <c r="O25" s="40"/>
+      <c r="P25" s="40"/>
+      <c r="Q25" s="40"/>
+      <c r="R25" s="40"/>
+      <c r="S25" s="40"/>
+      <c r="T25" s="40"/>
+      <c r="U25" s="40"/>
     </row>
     <row r="26" spans="1:21">
-      <c r="A26" s="37"/>
-      <c r="B26" s="37"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="37"/>
-      <c r="I26" s="37"/>
-      <c r="J26" s="37"/>
-      <c r="K26" s="37"/>
-      <c r="L26" s="37"/>
-      <c r="M26" s="37"/>
-      <c r="N26" s="37"/>
-      <c r="O26" s="37"/>
-      <c r="P26" s="37"/>
-      <c r="Q26" s="37"/>
-      <c r="R26" s="37"/>
-      <c r="S26" s="37"/>
-      <c r="T26" s="37"/>
-      <c r="U26" s="37"/>
+      <c r="A26" s="40"/>
+      <c r="B26" s="40"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="40"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="40"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="40"/>
+      <c r="L26" s="40"/>
+      <c r="M26" s="40"/>
+      <c r="N26" s="40"/>
+      <c r="O26" s="40"/>
+      <c r="P26" s="40"/>
+      <c r="Q26" s="40"/>
+      <c r="R26" s="40"/>
+      <c r="S26" s="40"/>
+      <c r="T26" s="40"/>
+      <c r="U26" s="40"/>
     </row>
     <row r="27" spans="1:21">
-      <c r="A27" s="37"/>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
-      <c r="K27" s="37"/>
-      <c r="L27" s="37"/>
-      <c r="M27" s="37"/>
-      <c r="N27" s="37"/>
-      <c r="O27" s="37"/>
-      <c r="P27" s="37"/>
-      <c r="Q27" s="37"/>
-      <c r="R27" s="37"/>
-      <c r="S27" s="37"/>
-      <c r="T27" s="37"/>
-      <c r="U27" s="37"/>
+      <c r="A27" s="40"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="40"/>
+      <c r="H27" s="40"/>
+      <c r="I27" s="40"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="40"/>
+      <c r="L27" s="40"/>
+      <c r="M27" s="40"/>
+      <c r="N27" s="40"/>
+      <c r="O27" s="40"/>
+      <c r="P27" s="40"/>
+      <c r="Q27" s="40"/>
+      <c r="R27" s="40"/>
+      <c r="S27" s="40"/>
+      <c r="T27" s="40"/>
+      <c r="U27" s="40"/>
     </row>
     <row r="28" spans="1:21">
-      <c r="A28" s="37"/>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
-      <c r="K28" s="37"/>
-      <c r="L28" s="37"/>
-      <c r="M28" s="37"/>
-      <c r="N28" s="37"/>
-      <c r="O28" s="37"/>
-      <c r="P28" s="37"/>
-      <c r="Q28" s="37"/>
-      <c r="R28" s="37"/>
-      <c r="S28" s="37"/>
-      <c r="T28" s="37"/>
-      <c r="U28" s="37"/>
+      <c r="A28" s="40"/>
+      <c r="B28" s="40"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="40"/>
+      <c r="H28" s="40"/>
+      <c r="I28" s="40"/>
+      <c r="J28" s="40"/>
+      <c r="K28" s="40"/>
+      <c r="L28" s="40"/>
+      <c r="M28" s="40"/>
+      <c r="N28" s="40"/>
+      <c r="O28" s="40"/>
+      <c r="P28" s="40"/>
+      <c r="Q28" s="40"/>
+      <c r="R28" s="40"/>
+      <c r="S28" s="40"/>
+      <c r="T28" s="40"/>
+      <c r="U28" s="40"/>
     </row>
     <row r="29" spans="1:21">
-      <c r="A29" s="37"/>
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="37"/>
-      <c r="J29" s="37"/>
-      <c r="K29" s="37"/>
-      <c r="L29" s="37"/>
-      <c r="M29" s="37"/>
-      <c r="N29" s="37"/>
-      <c r="O29" s="37"/>
-      <c r="P29" s="37"/>
-      <c r="Q29" s="37"/>
-      <c r="R29" s="37"/>
-      <c r="S29" s="37"/>
-      <c r="T29" s="37"/>
-      <c r="U29" s="37"/>
+      <c r="A29" s="40"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
+      <c r="K29" s="40"/>
+      <c r="L29" s="40"/>
+      <c r="M29" s="40"/>
+      <c r="N29" s="40"/>
+      <c r="O29" s="40"/>
+      <c r="P29" s="40"/>
+      <c r="Q29" s="40"/>
+      <c r="R29" s="40"/>
+      <c r="S29" s="40"/>
+      <c r="T29" s="40"/>
+      <c r="U29" s="40"/>
     </row>
     <row r="30" spans="1:21">
-      <c r="A30" s="37"/>
-      <c r="B30" s="37"/>
-      <c r="C30" s="37"/>
-      <c r="D30" s="37"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="37"/>
-      <c r="G30" s="37"/>
-      <c r="H30" s="37"/>
-      <c r="I30" s="37"/>
-      <c r="J30" s="37"/>
-      <c r="K30" s="37"/>
-      <c r="L30" s="37"/>
-      <c r="M30" s="37"/>
-      <c r="N30" s="37"/>
-      <c r="O30" s="37"/>
-      <c r="P30" s="37"/>
-      <c r="Q30" s="37"/>
-      <c r="R30" s="37"/>
-      <c r="S30" s="37"/>
-      <c r="T30" s="37"/>
-      <c r="U30" s="37"/>
+      <c r="A30" s="40"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
+      <c r="K30" s="40"/>
+      <c r="L30" s="40"/>
+      <c r="M30" s="40"/>
+      <c r="N30" s="40"/>
+      <c r="O30" s="40"/>
+      <c r="P30" s="40"/>
+      <c r="Q30" s="40"/>
+      <c r="R30" s="40"/>
+      <c r="S30" s="40"/>
+      <c r="T30" s="40"/>
+      <c r="U30" s="40"/>
     </row>
     <row r="31" spans="1:21">
-      <c r="A31" s="37"/>
-      <c r="B31" s="37"/>
-      <c r="C31" s="37"/>
-      <c r="D31" s="37"/>
-      <c r="E31" s="37"/>
-      <c r="F31" s="37"/>
-      <c r="G31" s="37"/>
-      <c r="H31" s="37"/>
-      <c r="I31" s="37"/>
-      <c r="J31" s="37"/>
-      <c r="K31" s="37"/>
-      <c r="L31" s="37"/>
-      <c r="M31" s="37"/>
-      <c r="N31" s="37"/>
-      <c r="O31" s="37"/>
-      <c r="P31" s="37"/>
-      <c r="Q31" s="37"/>
-      <c r="R31" s="37"/>
-      <c r="S31" s="37"/>
-      <c r="T31" s="37"/>
-      <c r="U31" s="37"/>
+      <c r="A31" s="40"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="40"/>
+      <c r="K31" s="40"/>
+      <c r="L31" s="40"/>
+      <c r="M31" s="40"/>
+      <c r="N31" s="40"/>
+      <c r="O31" s="40"/>
+      <c r="P31" s="40"/>
+      <c r="Q31" s="40"/>
+      <c r="R31" s="40"/>
+      <c r="S31" s="40"/>
+      <c r="T31" s="40"/>
+      <c r="U31" s="40"/>
     </row>
     <row r="32" spans="1:21">
-      <c r="A32" s="37"/>
-      <c r="B32" s="37"/>
-      <c r="C32" s="37"/>
-      <c r="D32" s="37"/>
-      <c r="E32" s="37"/>
-      <c r="F32" s="37"/>
-      <c r="G32" s="37"/>
-      <c r="H32" s="37"/>
-      <c r="I32" s="37"/>
-      <c r="J32" s="37"/>
-      <c r="K32" s="37"/>
-      <c r="L32" s="37"/>
-      <c r="M32" s="37"/>
-      <c r="N32" s="37"/>
-      <c r="O32" s="37"/>
-      <c r="P32" s="37"/>
-      <c r="Q32" s="37"/>
-      <c r="R32" s="37"/>
-      <c r="S32" s="37"/>
-      <c r="T32" s="37"/>
-      <c r="U32" s="37"/>
+      <c r="A32" s="40"/>
+      <c r="B32" s="40"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="40"/>
+      <c r="E32" s="40"/>
+      <c r="F32" s="40"/>
+      <c r="G32" s="40"/>
+      <c r="H32" s="40"/>
+      <c r="I32" s="40"/>
+      <c r="J32" s="40"/>
+      <c r="K32" s="40"/>
+      <c r="L32" s="40"/>
+      <c r="M32" s="40"/>
+      <c r="N32" s="40"/>
+      <c r="O32" s="40"/>
+      <c r="P32" s="40"/>
+      <c r="Q32" s="40"/>
+      <c r="R32" s="40"/>
+      <c r="S32" s="40"/>
+      <c r="T32" s="40"/>
+      <c r="U32" s="40"/>
     </row>
     <row r="33" spans="1:21">
-      <c r="A33" s="37"/>
-      <c r="B33" s="37"/>
-      <c r="C33" s="37"/>
-      <c r="D33" s="37"/>
-      <c r="E33" s="37"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="37"/>
-      <c r="H33" s="37"/>
-      <c r="I33" s="37"/>
-      <c r="J33" s="37"/>
-      <c r="K33" s="37"/>
-      <c r="L33" s="37"/>
-      <c r="M33" s="37"/>
-      <c r="N33" s="37"/>
-      <c r="O33" s="37"/>
-      <c r="P33" s="37"/>
-      <c r="Q33" s="37"/>
-      <c r="R33" s="37"/>
-      <c r="S33" s="37"/>
-      <c r="T33" s="37"/>
-      <c r="U33" s="37"/>
+      <c r="A33" s="40"/>
+      <c r="B33" s="40"/>
+      <c r="C33" s="40"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="40"/>
+      <c r="F33" s="40"/>
+      <c r="G33" s="40"/>
+      <c r="H33" s="40"/>
+      <c r="I33" s="40"/>
+      <c r="J33" s="40"/>
+      <c r="K33" s="40"/>
+      <c r="L33" s="40"/>
+      <c r="M33" s="40"/>
+      <c r="N33" s="40"/>
+      <c r="O33" s="40"/>
+      <c r="P33" s="40"/>
+      <c r="Q33" s="40"/>
+      <c r="R33" s="40"/>
+      <c r="S33" s="40"/>
+      <c r="T33" s="40"/>
+      <c r="U33" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A23:G23"/>
+    <mergeCell ref="H23:N23"/>
+    <mergeCell ref="O23:U23"/>
+    <mergeCell ref="A24:G33"/>
+    <mergeCell ref="H24:N33"/>
+    <mergeCell ref="O24:U33"/>
+    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="H12:N12"/>
+    <mergeCell ref="O12:U12"/>
+    <mergeCell ref="A13:G22"/>
+    <mergeCell ref="H13:N22"/>
+    <mergeCell ref="O13:U22"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="H1:N1"/>
     <mergeCell ref="O1:U1"/>
     <mergeCell ref="A2:G11"/>
     <mergeCell ref="H2:N11"/>
     <mergeCell ref="O2:U11"/>
-    <mergeCell ref="A12:G12"/>
-    <mergeCell ref="H12:N12"/>
-    <mergeCell ref="O12:U12"/>
-    <mergeCell ref="A13:G22"/>
-    <mergeCell ref="H13:N22"/>
-    <mergeCell ref="O13:U22"/>
-    <mergeCell ref="A23:G23"/>
-    <mergeCell ref="H23:N23"/>
-    <mergeCell ref="O23:U23"/>
-    <mergeCell ref="A24:G33"/>
-    <mergeCell ref="H24:N33"/>
-    <mergeCell ref="O24:U33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3151,8 +3208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3165,310 +3222,310 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="34" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="33" t="s">
         <v>128</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="E2" s="39">
+      <c r="E2" s="33">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="33" t="s">
         <v>129</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="33" t="s">
         <v>104</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="D3" s="39" t="s">
+      <c r="D3" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="E3" s="39">
+      <c r="E3" s="33">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="33" t="s">
         <v>130</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="33" t="s">
         <v>122</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="33" t="s">
         <v>112</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="D4" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="E4" s="39">
+      <c r="E4" s="33">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="33" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="33" t="s">
         <v>121</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="D5" s="39" t="s">
+      <c r="D5" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="E5" s="39">
+      <c r="E5" s="33">
         <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="C6" s="39" t="s">
+      <c r="C6" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="D6" s="39" t="s">
+      <c r="D6" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="33">
         <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="33" t="s">
         <v>133</v>
       </c>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="33" t="s">
         <v>124</v>
       </c>
-      <c r="D7" s="39" t="s">
+      <c r="D7" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="33">
         <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="33" t="s">
         <v>134</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="33" t="s">
         <v>126</v>
       </c>
-      <c r="C8" s="39" t="s">
+      <c r="C8" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="D8" s="39" t="s">
+      <c r="D8" s="33" t="s">
         <v>127</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="33">
         <v>250</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="33" t="s">
         <v>135</v>
       </c>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="C9" s="39" t="s">
+      <c r="C9" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39">
+      <c r="D9" s="33"/>
+      <c r="E9" s="33">
         <v>253</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="33" t="s">
         <v>151</v>
       </c>
-      <c r="C10" s="39" t="s">
+      <c r="C10" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39">
+      <c r="D10" s="33"/>
+      <c r="E10" s="33">
         <v>253</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="33" t="s">
         <v>157</v>
       </c>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39">
+      <c r="D11" s="33"/>
+      <c r="E11" s="33">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="33" t="s">
         <v>156</v>
       </c>
-      <c r="C12" s="39" t="s">
+      <c r="C12" s="33" t="s">
         <v>158</v>
       </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39">
+      <c r="D12" s="33"/>
+      <c r="E12" s="33">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="B14" s="39"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="B15" s="39"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="39"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="33" t="s">
         <v>143</v>
       </c>
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="B18" s="39"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="39" t="s">
+      <c r="A19" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="39" t="s">
+      <c r="A20" s="33" t="s">
         <v>146</v>
       </c>
-      <c r="B20" s="39"/>
-      <c r="C20" s="39"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="39"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="33" t="s">
         <v>147</v>
       </c>
-      <c r="B21" s="39"/>
-      <c r="C21" s="39"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="39"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="33" t="s">
         <v>148</v>
       </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="39"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="39"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="33" t="s">
         <v>149</v>
       </c>
-      <c r="B23" s="39"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="41" t="s">
+      <c r="A24" s="35" t="s">
         <v>153</v>
       </c>
-      <c r="B24" s="41" t="s">
+      <c r="B24" s="35" t="s">
         <v>154</v>
       </c>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="41">
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="35">
         <v>254</v>
       </c>
     </row>
@@ -3477,4 +3534,30 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="V5:V6"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="W11" sqref="W11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="5" spans="22:22">
+      <c r="V5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="6" spans="22:22">
+      <c r="V6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>